<commit_message>
Still fixing all problems due to change of level system
</commit_message>
<xml_diff>
--- a/public/Level.xlsx
+++ b/public/Level.xlsx
@@ -8,15 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kevin Zeugs\Studium\Free_Projects\idle_alphabet\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08DEA8A8-CB82-4CD7-9B97-6FF6F281C0A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C308A14-83C8-4D3C-B86E-6D525BE5D9BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-135" windowWidth="38640" windowHeight="21240" xr2:uid="{EE7CB22D-DBB3-4CC5-A134-0A5565C2D036}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{EE7CB22D-DBB3-4CC5-A134-0A5565C2D036}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="769" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="773" uniqueCount="57">
   <si>
     <t>Basisliste</t>
   </si>
@@ -200,11 +199,23 @@
   <si>
     <t>Costs Slot 4</t>
   </si>
+  <si>
+    <t>Speed</t>
+  </si>
+  <si>
+    <t>Rate</t>
+  </si>
+  <si>
+    <t>Rate Init</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="#,##0.0000000000000000"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -320,7 +331,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -333,12 +344,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -355,6 +362,7 @@
     </xf>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -671,18 +679,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F719A59D-A330-4459-AA9A-D2893BAE4388}">
   <dimension ref="A1:FE117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="F118" sqref="F118"/>
+    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="K66" sqref="K66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="54.7109375" customWidth="1"/>
-    <col min="4" max="4" width="53.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="51.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="41" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" customWidth="1"/>
+    <col min="7" max="7" width="27.140625" customWidth="1"/>
+    <col min="9" max="9" width="26.5703125" customWidth="1"/>
+    <col min="10" max="10" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="4" customWidth="1"/>
     <col min="18" max="18" width="4" customWidth="1"/>
     <col min="24" max="24" width="4" customWidth="1"/>
@@ -801,25 +812,22 @@
     </row>
     <row r="2" spans="1:161" x14ac:dyDescent="0.25">
       <c r="A2" s="7"/>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="9"/>
+      <c r="E2" s="8"/>
     </row>
     <row r="3" spans="1:161" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="8" t="s">
         <v>5</v>
       </c>
       <c r="G3" t="s">
@@ -1214,15 +1222,15 @@
       </c>
     </row>
     <row r="4" spans="1:161" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="12"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="10"/>
       <c r="G4" s="2" t="s">
         <v>6</v>
       </c>
@@ -1437,17 +1445,16 @@
       <c r="FE4" s="2"/>
     </row>
     <row r="5" spans="1:161" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="8"/>
-      <c r="E5" s="12"/>
+      <c r="E5" s="10"/>
       <c r="G5" s="2" t="s">
         <v>7</v>
       </c>
@@ -1662,19 +1669,19 @@
       <c r="FE5" s="2"/>
     </row>
     <row r="6" spans="1:161" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="11" t="s">
+      <c r="D6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="9"/>
+      <c r="E6" s="8"/>
       <c r="G6" s="2" t="s">
         <v>8</v>
       </c>
@@ -1917,19 +1924,19 @@
       </c>
     </row>
     <row r="7" spans="1:161" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="11" t="s">
+      <c r="D7" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E7" s="12" t="s">
+      <c r="E7" s="10" t="s">
         <v>15</v>
       </c>
       <c r="G7" s="2" t="s">
@@ -2226,19 +2233,19 @@
       </c>
     </row>
     <row r="8" spans="1:161" x14ac:dyDescent="0.25">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="11" t="s">
+      <c r="D8" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E8" s="12" t="s">
+      <c r="E8" s="10" t="s">
         <v>19</v>
       </c>
       <c r="G8" s="2" t="s">
@@ -2537,19 +2544,19 @@
       <c r="FE8" s="2"/>
     </row>
     <row r="9" spans="1:161" x14ac:dyDescent="0.25">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="11" t="s">
+      <c r="D9" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E9" s="12" t="s">
+      <c r="E9" s="10" t="s">
         <v>21</v>
       </c>
       <c r="G9" s="2" t="s">
@@ -2850,19 +2857,19 @@
       <c r="FE9" s="2"/>
     </row>
     <row r="10" spans="1:161" x14ac:dyDescent="0.25">
-      <c r="A10" s="10" t="s">
+      <c r="A10" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C10" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="11" t="s">
+      <c r="D10" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E10" s="12" t="s">
+      <c r="E10" s="10" t="s">
         <v>22</v>
       </c>
       <c r="G10" s="2" t="s">
@@ -3157,19 +3164,19 @@
       <c r="FE10" s="2"/>
     </row>
     <row r="11" spans="1:161" x14ac:dyDescent="0.25">
-      <c r="A11" s="13" t="s">
+      <c r="A11" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="14" t="s">
+      <c r="B11" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="14" t="s">
+      <c r="C11" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="D11" s="14" t="s">
+      <c r="D11" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="E11" s="15" t="s">
+      <c r="E11" s="13" t="s">
         <v>23</v>
       </c>
       <c r="G11" s="2" t="s">
@@ -3482,2421 +3489,3385 @@
       <c r="F16" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="17">
+      <c r="G16" t="s">
+        <v>54</v>
+      </c>
+      <c r="H16" t="s">
+        <v>49</v>
+      </c>
+      <c r="I16" t="s">
+        <v>55</v>
+      </c>
+      <c r="J16" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="15">
         <v>1</v>
       </c>
-      <c r="B17" s="16"/>
-      <c r="C17" s="17">
+      <c r="B17" s="14"/>
+      <c r="C17" s="15">
         <v>10</v>
       </c>
-      <c r="D17" s="17"/>
-      <c r="E17" s="17"/>
-      <c r="F17" s="17"/>
-      <c r="G17" s="17"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="17">
+      <c r="D17" s="15"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="15"/>
+      <c r="G17" s="16">
+        <v>1</v>
+      </c>
+      <c r="I17">
+        <v>1</v>
+      </c>
+      <c r="J17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="15">
         <f>A17+1</f>
         <v>2</v>
       </c>
-      <c r="B18" s="16">
+      <c r="B18" s="14">
         <v>1.2</v>
       </c>
-      <c r="C18" s="17">
+      <c r="C18" s="15">
         <f>ROUND((C17*(B18^A18)), 0)</f>
         <v>14</v>
       </c>
-      <c r="D18" s="17"/>
-      <c r="E18" s="17"/>
-      <c r="F18" s="17"/>
-      <c r="G18" s="17"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="17">
+      <c r="D18" s="15"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="16">
+        <f>G17/(H18^A17)</f>
+        <v>0.95238095238095233</v>
+      </c>
+      <c r="H18">
+        <v>1.05</v>
+      </c>
+      <c r="I18" s="14">
+        <f>J18*(B18^A17)</f>
+        <v>1.2</v>
+      </c>
+      <c r="J18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="15">
         <f t="shared" ref="A19:A82" si="0">A18+1</f>
         <v>3</v>
       </c>
-      <c r="B19" s="16">
+      <c r="B19" s="14">
         <v>1.2</v>
       </c>
-      <c r="C19" s="17">
+      <c r="C19" s="15">
         <f>ROUND((C17*(B19^A19)), 0)</f>
         <v>17</v>
       </c>
-      <c r="D19" s="17"/>
-      <c r="E19" s="17"/>
-      <c r="F19" s="17"/>
-      <c r="G19" s="17"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="17">
+      <c r="D19" s="15"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="15"/>
+      <c r="G19" s="16">
+        <f>G17/(H19^A18)</f>
+        <v>0.90702947845804982</v>
+      </c>
+      <c r="H19">
+        <v>1.05</v>
+      </c>
+      <c r="I19" s="14">
+        <f t="shared" ref="I19:I66" si="1">J19*(B19^A18)</f>
+        <v>1.44</v>
+      </c>
+      <c r="J19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="15">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B20" s="16">
+      <c r="B20" s="14">
         <v>1.2</v>
       </c>
-      <c r="C20" s="17">
+      <c r="C20" s="15">
         <f>ROUND((C17*(B20^A20)), 0)</f>
         <v>21</v>
       </c>
-      <c r="D20" s="17"/>
-      <c r="E20" s="17"/>
-      <c r="F20" s="17"/>
-      <c r="G20" s="17"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="17">
+      <c r="D20" s="15"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="15"/>
+      <c r="G20" s="16">
+        <f>G17/(H20^A19)</f>
+        <v>0.86383759853147601</v>
+      </c>
+      <c r="H20">
+        <v>1.05</v>
+      </c>
+      <c r="I20" s="14">
+        <f t="shared" si="1"/>
+        <v>1.728</v>
+      </c>
+      <c r="J20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="15">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B21" s="16">
+      <c r="B21" s="14">
         <v>1.2</v>
       </c>
-      <c r="C21" s="17">
+      <c r="C21" s="15">
         <f>ROUND((C17*(B21^A21)), 0)</f>
         <v>25</v>
       </c>
-      <c r="D21" s="17"/>
-      <c r="E21" s="17"/>
-      <c r="F21" s="17"/>
-      <c r="G21" s="17"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="17">
+      <c r="D21" s="15"/>
+      <c r="E21" s="15"/>
+      <c r="F21" s="15"/>
+      <c r="G21" s="16">
+        <f>G17/(H21^A20)</f>
+        <v>0.82270247479188197</v>
+      </c>
+      <c r="H21">
+        <v>1.05</v>
+      </c>
+      <c r="I21" s="14">
+        <f t="shared" si="1"/>
+        <v>2.0735999999999999</v>
+      </c>
+      <c r="J21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="15">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B22" s="16">
+      <c r="B22" s="14">
         <v>1.2</v>
       </c>
-      <c r="C22" s="17">
+      <c r="C22" s="15">
         <f>ROUND((C17*(B22^A22)), 0)</f>
         <v>30</v>
       </c>
-      <c r="D22" s="17"/>
-      <c r="E22" s="17"/>
-      <c r="F22" s="17"/>
-      <c r="G22" s="17"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="17">
+      <c r="D22" s="15"/>
+      <c r="E22" s="15"/>
+      <c r="F22" s="15"/>
+      <c r="G22" s="16">
+        <f>G17/(H22^A21)</f>
+        <v>0.78352616646845896</v>
+      </c>
+      <c r="H22">
+        <v>1.05</v>
+      </c>
+      <c r="I22" s="14">
+        <f t="shared" si="1"/>
+        <v>2.4883199999999999</v>
+      </c>
+      <c r="J22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="15">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B23" s="16">
+      <c r="B23" s="14">
         <v>1.2</v>
       </c>
-      <c r="C23" s="17">
+      <c r="C23" s="15">
         <f>ROUND((C17*(B23^A23)), 0)</f>
         <v>36</v>
       </c>
-      <c r="D23" s="17"/>
-      <c r="E23" s="17"/>
-      <c r="F23" s="17"/>
-      <c r="G23" s="17"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="17">
+      <c r="D23" s="15"/>
+      <c r="E23" s="15"/>
+      <c r="F23" s="15"/>
+      <c r="G23" s="16">
+        <f>G17/(H23^A22)</f>
+        <v>0.74621539663662761</v>
+      </c>
+      <c r="H23">
+        <v>1.05</v>
+      </c>
+      <c r="I23" s="14">
+        <f t="shared" si="1"/>
+        <v>2.9859839999999997</v>
+      </c>
+      <c r="J23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" s="15">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="B24" s="16">
+      <c r="B24" s="14">
         <v>1.2</v>
       </c>
-      <c r="C24" s="17">
+      <c r="C24" s="15">
         <f>ROUND((C17*(B24^A24)), 0)</f>
         <v>43</v>
       </c>
-      <c r="D24" s="17"/>
-      <c r="E24" s="17"/>
-      <c r="F24" s="17"/>
-      <c r="G24" s="17"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="17">
+      <c r="D24" s="15"/>
+      <c r="E24" s="15"/>
+      <c r="F24" s="15"/>
+      <c r="G24" s="16">
+        <f>G17/(H24^A23)</f>
+        <v>0.71068133013012147</v>
+      </c>
+      <c r="H24">
+        <v>1.05</v>
+      </c>
+      <c r="I24" s="14">
+        <f t="shared" si="1"/>
+        <v>3.5831807999999996</v>
+      </c>
+      <c r="J24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="15">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="B25" s="16">
+      <c r="B25" s="14">
         <v>1.2</v>
       </c>
-      <c r="C25" s="17">
+      <c r="C25" s="15">
         <f>ROUND((C17*(B25^A25)), 0)</f>
         <v>52</v>
       </c>
-      <c r="D25" s="17"/>
-      <c r="E25" s="17"/>
-      <c r="F25" s="17"/>
-      <c r="G25" s="17"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="17">
+      <c r="D25" s="15"/>
+      <c r="E25" s="15"/>
+      <c r="F25" s="15"/>
+      <c r="G25" s="16">
+        <f>G17/(H25^A24)</f>
+        <v>0.67683936202868722</v>
+      </c>
+      <c r="H25">
+        <v>1.05</v>
+      </c>
+      <c r="I25" s="14">
+        <f t="shared" si="1"/>
+        <v>4.2998169599999994</v>
+      </c>
+      <c r="J25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" s="15">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="B26" s="16">
+      <c r="B26" s="14">
         <v>1.2</v>
       </c>
-      <c r="C26" s="17">
+      <c r="C26" s="15">
         <f>ROUND((C17*(B26^A26)), 0)</f>
         <v>62</v>
       </c>
-      <c r="D26" s="17">
+      <c r="D26" s="15">
         <v>10</v>
       </c>
-      <c r="E26" s="17"/>
-      <c r="F26" s="17"/>
-      <c r="G26" s="17"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="17">
+      <c r="E26" s="15"/>
+      <c r="F26" s="15"/>
+      <c r="G26" s="16">
+        <f>G17/(H26^A25)</f>
+        <v>0.64460891621779726</v>
+      </c>
+      <c r="H26">
+        <v>1.05</v>
+      </c>
+      <c r="I26" s="14">
+        <f t="shared" si="1"/>
+        <v>5.1597803519999994</v>
+      </c>
+      <c r="J26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" s="15">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="B27" s="16">
+      <c r="B27" s="14">
         <v>1.25</v>
       </c>
-      <c r="C27" s="17">
+      <c r="C27" s="15">
         <f>ROUND((C26*(B27^A27)), 0)</f>
         <v>722</v>
       </c>
-      <c r="D27" s="17">
+      <c r="D27" s="15">
         <f>ROUND((D26*(B27^A27)), 0)</f>
         <v>116</v>
       </c>
-      <c r="E27" s="17"/>
-      <c r="F27" s="17"/>
-      <c r="G27" s="17"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="17">
+      <c r="E27" s="15"/>
+      <c r="F27" s="15"/>
+      <c r="G27" s="16">
+        <f>G26/(H27^A26)</f>
+        <v>0.52880382850363639</v>
+      </c>
+      <c r="H27">
+        <v>1.02</v>
+      </c>
+      <c r="I27" s="14">
+        <f t="shared" si="1"/>
+        <v>48.056244850158691</v>
+      </c>
+      <c r="J27" s="14">
+        <v>5.16</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" s="15">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="B28" s="16">
+      <c r="B28" s="14">
         <v>1.25</v>
       </c>
-      <c r="C28" s="17">
+      <c r="C28" s="15">
         <f>ROUND((C26*(B28^A28)), 0)</f>
         <v>902</v>
       </c>
-      <c r="D28" s="17">
+      <c r="D28" s="15">
         <f>ROUND((D26*(B28^A28)), 0)</f>
         <v>146</v>
       </c>
-      <c r="E28" s="17"/>
-      <c r="F28" s="17"/>
-      <c r="G28" s="17"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="17">
+      <c r="E28" s="15"/>
+      <c r="F28" s="15"/>
+      <c r="G28" s="16">
+        <f>G26/(H28^A27)</f>
+        <v>0.51843512598395736</v>
+      </c>
+      <c r="H28">
+        <v>1.02</v>
+      </c>
+      <c r="I28" s="14">
+        <f t="shared" si="1"/>
+        <v>60.070306062698364</v>
+      </c>
+      <c r="J28" s="14">
+        <v>5.16</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" s="15">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="B29" s="16">
+      <c r="B29" s="14">
         <v>1.25</v>
       </c>
-      <c r="C29" s="17">
+      <c r="C29" s="15">
         <f>ROUND((C26*(B29^A29)), 0)</f>
         <v>1128</v>
       </c>
-      <c r="D29" s="17">
+      <c r="D29" s="15">
         <f>ROUND((D26*(B29^A29)), 0)</f>
         <v>182</v>
       </c>
-      <c r="E29" s="17"/>
-      <c r="F29" s="17"/>
-      <c r="G29" s="17"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="17">
+      <c r="E29" s="15"/>
+      <c r="F29" s="15"/>
+      <c r="G29" s="16">
+        <f>G26/(H29^A28)</f>
+        <v>0.50826973135682085</v>
+      </c>
+      <c r="H29">
+        <v>1.02</v>
+      </c>
+      <c r="I29" s="14">
+        <f t="shared" si="1"/>
+        <v>75.087882578372955</v>
+      </c>
+      <c r="J29" s="14">
+        <v>5.16</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" s="15">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="B30" s="16">
+      <c r="B30" s="14">
         <v>1.25</v>
       </c>
-      <c r="C30" s="17">
+      <c r="C30" s="15">
         <f>ROUND((C26*(B30^A30)), 0)</f>
         <v>1410</v>
       </c>
-      <c r="D30" s="17">
+      <c r="D30" s="15">
         <f>ROUND((D26*(B30^A30)), 0)</f>
         <v>227</v>
       </c>
-      <c r="E30" s="17"/>
-      <c r="F30" s="17"/>
-      <c r="G30" s="17"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="17">
+      <c r="E30" s="15"/>
+      <c r="F30" s="15"/>
+      <c r="G30" s="16">
+        <f>G26/(H30^A29)</f>
+        <v>0.49830365819296163</v>
+      </c>
+      <c r="H30">
+        <v>1.02</v>
+      </c>
+      <c r="I30" s="14">
+        <f t="shared" si="1"/>
+        <v>93.859853222966194</v>
+      </c>
+      <c r="J30" s="14">
+        <v>5.16</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" s="15">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="B31" s="16">
+      <c r="B31" s="14">
         <v>1.25</v>
       </c>
-      <c r="C31" s="17">
+      <c r="C31" s="15">
         <f>ROUND((C26*(B31^A31)), 0)</f>
         <v>1762</v>
       </c>
-      <c r="D31" s="17">
+      <c r="D31" s="15">
         <f>ROUND((D26*(B31^A31)), 0)</f>
         <v>284</v>
       </c>
-      <c r="E31" s="17"/>
-      <c r="F31" s="17"/>
-      <c r="G31" s="17"/>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="17">
+      <c r="E31" s="15"/>
+      <c r="F31" s="15"/>
+      <c r="G31" s="16">
+        <f>G26/(H31^A30)</f>
+        <v>0.48853299822839374</v>
+      </c>
+      <c r="H31">
+        <v>1.02</v>
+      </c>
+      <c r="I31" s="14">
+        <f t="shared" si="1"/>
+        <v>117.32481652870774</v>
+      </c>
+      <c r="J31" s="14">
+        <v>5.16</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" s="15">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="B32" s="16">
+      <c r="B32" s="14">
         <v>1.25</v>
       </c>
-      <c r="C32" s="17">
+      <c r="C32" s="15">
         <f>ROUND((C26*(B32^A32)), 0)</f>
         <v>2203</v>
       </c>
-      <c r="D32" s="17">
+      <c r="D32" s="15">
         <f>ROUND((D26*(B32^A32)), 0)</f>
         <v>355</v>
       </c>
-      <c r="E32" s="17"/>
-      <c r="F32" s="17"/>
-      <c r="G32" s="17"/>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="17">
+      <c r="E32" s="15"/>
+      <c r="F32" s="15"/>
+      <c r="G32" s="16">
+        <f>G26/(H32^A31)</f>
+        <v>0.47895391983175867</v>
+      </c>
+      <c r="H32">
+        <v>1.02</v>
+      </c>
+      <c r="I32" s="14">
+        <f t="shared" si="1"/>
+        <v>146.65602066088468</v>
+      </c>
+      <c r="J32" s="14">
+        <v>5.16</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" s="15">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="B33" s="16">
+      <c r="B33" s="14">
         <v>1.25</v>
       </c>
-      <c r="C33" s="17">
+      <c r="C33" s="15">
         <f>ROUND((C26*(B33^A33)), 0)</f>
         <v>2753</v>
       </c>
-      <c r="D33" s="17">
+      <c r="D33" s="15">
         <f>ROUND((D26*(B33^A33)), 0)</f>
         <v>444</v>
       </c>
-      <c r="E33" s="17"/>
-      <c r="F33" s="17"/>
-      <c r="G33" s="17"/>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="17">
+      <c r="E33" s="15"/>
+      <c r="F33" s="15"/>
+      <c r="G33" s="16">
+        <f>G26/(H33^A32)</f>
+        <v>0.46956266650172412</v>
+      </c>
+      <c r="H33">
+        <v>1.02</v>
+      </c>
+      <c r="I33" s="14">
+        <f t="shared" si="1"/>
+        <v>183.32002582610585</v>
+      </c>
+      <c r="J33" s="14">
+        <v>5.16</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" s="15">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="B34" s="16">
+      <c r="B34" s="14">
         <v>1.25</v>
       </c>
-      <c r="C34" s="17">
+      <c r="C34" s="15">
         <f>ROUND((C26*(B34^A34)), 0)</f>
         <v>3442</v>
       </c>
-      <c r="D34" s="17">
+      <c r="D34" s="15">
         <f>ROUND((D26*(B34^A34)), 0)</f>
         <v>555</v>
       </c>
-      <c r="E34" s="17"/>
-      <c r="F34" s="17"/>
-      <c r="G34" s="17"/>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="17">
+      <c r="E34" s="15"/>
+      <c r="F34" s="15"/>
+      <c r="G34" s="16">
+        <f>G26/(H34^A33)</f>
+        <v>0.46035555539384715</v>
+      </c>
+      <c r="H34">
+        <v>1.02</v>
+      </c>
+      <c r="I34" s="14">
+        <f t="shared" si="1"/>
+        <v>229.15003228263231</v>
+      </c>
+      <c r="J34" s="14">
+        <v>5.16</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35" s="15">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="B35" s="16">
+      <c r="B35" s="14">
         <v>1.25</v>
       </c>
-      <c r="C35" s="17">
+      <c r="C35" s="15">
         <f>ROUND((C26*(B35^A35)), 0)</f>
         <v>4302</v>
       </c>
-      <c r="D35" s="17">
+      <c r="D35" s="15">
         <f>ROUND((D26*(B35^A35)), 0)</f>
         <v>694</v>
       </c>
-      <c r="E35" s="17"/>
-      <c r="F35" s="17"/>
-      <c r="G35" s="17"/>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="17">
+      <c r="E35" s="15"/>
+      <c r="F35" s="15"/>
+      <c r="G35" s="16">
+        <f>G26/(H35^A34)</f>
+        <v>0.45132897587632076</v>
+      </c>
+      <c r="H35">
+        <v>1.02</v>
+      </c>
+      <c r="I35" s="14">
+        <f t="shared" si="1"/>
+        <v>286.43754035329039</v>
+      </c>
+      <c r="J35" s="14">
+        <v>5.16</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A36" s="15">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="B36" s="16">
+      <c r="B36" s="14">
         <v>1.25</v>
       </c>
-      <c r="C36" s="17">
+      <c r="C36" s="15">
         <f>ROUND((C26*(B36^A36)), 0)</f>
         <v>5378</v>
       </c>
-      <c r="D36" s="17">
+      <c r="D36" s="15">
         <f>ROUND((D26*(B36^A36)), 0)</f>
         <v>867</v>
       </c>
-      <c r="E36" s="17"/>
-      <c r="F36" s="17"/>
-      <c r="G36" s="17"/>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="17">
+      <c r="E36" s="15"/>
+      <c r="F36" s="15"/>
+      <c r="G36" s="16">
+        <f>G26/(H36^A35)</f>
+        <v>0.44247938811403997</v>
+      </c>
+      <c r="H36">
+        <v>1.02</v>
+      </c>
+      <c r="I36" s="14">
+        <f t="shared" si="1"/>
+        <v>358.04692544161298</v>
+      </c>
+      <c r="J36" s="14">
+        <v>5.16</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37" s="15">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="B37" s="16">
+      <c r="B37" s="14">
         <v>1.25</v>
       </c>
-      <c r="C37" s="17">
+      <c r="C37" s="15">
         <f>ROUND((C26*(B37^A37)), 0)</f>
         <v>6722</v>
       </c>
-      <c r="D37" s="17">
+      <c r="D37" s="15">
         <f>ROUND((D26*(B37^A37)), 0)</f>
         <v>1084</v>
       </c>
-      <c r="E37" s="17"/>
-      <c r="F37" s="17"/>
-      <c r="G37" s="17"/>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="17">
+      <c r="E37" s="15"/>
+      <c r="F37" s="15"/>
+      <c r="G37" s="16">
+        <f>G26/(H37^A36)</f>
+        <v>0.43380332168043134</v>
+      </c>
+      <c r="H37">
+        <v>1.02</v>
+      </c>
+      <c r="I37" s="14">
+        <f t="shared" si="1"/>
+        <v>447.55865680201623</v>
+      </c>
+      <c r="J37" s="14">
+        <v>5.16</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A38" s="15">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="B38" s="16">
+      <c r="B38" s="14">
         <v>1.25</v>
       </c>
-      <c r="C38" s="17">
+      <c r="C38" s="15">
         <f>ROUND((C26*(B38^A38)), 0)</f>
         <v>8403</v>
       </c>
-      <c r="D38" s="17">
+      <c r="D38" s="15">
         <f>ROUND((D26*(B38^A38)), 0)</f>
         <v>1355</v>
       </c>
-      <c r="E38" s="17"/>
-      <c r="F38" s="17"/>
-      <c r="G38" s="17"/>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="17">
+      <c r="E38" s="15"/>
+      <c r="F38" s="15"/>
+      <c r="G38" s="16">
+        <f>G26/(H38^A37)</f>
+        <v>0.42529737419650132</v>
+      </c>
+      <c r="H38">
+        <v>1.02</v>
+      </c>
+      <c r="I38" s="14">
+        <f t="shared" si="1"/>
+        <v>559.44832100252029</v>
+      </c>
+      <c r="J38" s="14">
+        <v>5.16</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A39" s="15">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="B39" s="16">
+      <c r="B39" s="14">
         <v>1.25</v>
       </c>
-      <c r="C39" s="17">
+      <c r="C39" s="15">
         <f>ROUND((C26*(B39^A39)), 0)</f>
         <v>10503</v>
       </c>
-      <c r="D39" s="17">
+      <c r="D39" s="15">
         <f>ROUND((D26*(B39^A39)), 0)</f>
         <v>1694</v>
       </c>
-      <c r="E39" s="17"/>
-      <c r="F39" s="17"/>
-      <c r="G39" s="17"/>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="17">
+      <c r="E39" s="15"/>
+      <c r="F39" s="15"/>
+      <c r="G39" s="16">
+        <f>G26/(H39^A38)</f>
+        <v>0.41695820999656991</v>
+      </c>
+      <c r="H39">
+        <v>1.02</v>
+      </c>
+      <c r="I39" s="14">
+        <f t="shared" si="1"/>
+        <v>699.31040125315042</v>
+      </c>
+      <c r="J39" s="14">
+        <v>5.16</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A40" s="15">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="B40" s="16">
+      <c r="B40" s="14">
         <v>1.25</v>
       </c>
-      <c r="C40" s="17">
+      <c r="C40" s="15">
         <f>ROUND((C26*(B40^A40)), 0)</f>
         <v>13129</v>
       </c>
-      <c r="D40" s="17">
+      <c r="D40" s="15">
         <f>ROUND((D26*(B40^A40)), 0)</f>
         <v>2118</v>
       </c>
-      <c r="E40" s="17"/>
-      <c r="F40" s="17"/>
-      <c r="G40" s="17"/>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="17">
+      <c r="E40" s="15"/>
+      <c r="F40" s="15"/>
+      <c r="G40" s="16">
+        <f>G26/(H40^A39)</f>
+        <v>0.40878255882016662</v>
+      </c>
+      <c r="H40">
+        <v>1.02</v>
+      </c>
+      <c r="I40" s="14">
+        <f t="shared" si="1"/>
+        <v>874.13800156643788</v>
+      </c>
+      <c r="J40" s="14">
+        <v>5.16</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A41" s="15">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="B41" s="16">
+      <c r="B41" s="14">
         <v>1.25</v>
       </c>
-      <c r="C41" s="17">
+      <c r="C41" s="15">
         <f>ROUND((C26*(B41^A41)), 0)</f>
         <v>16411</v>
       </c>
-      <c r="D41" s="17">
+      <c r="D41" s="15">
         <f>ROUND((D26*(B41^A41)), 0)</f>
         <v>2647</v>
       </c>
-      <c r="E41" s="17">
+      <c r="E41" s="15">
         <v>10</v>
       </c>
-      <c r="F41" s="17"/>
-      <c r="G41" s="17"/>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="17">
+      <c r="F41" s="15"/>
+      <c r="G41" s="16">
+        <f>G26/(H41^A40)</f>
+        <v>0.40076721452957514</v>
+      </c>
+      <c r="H41">
+        <v>1.02</v>
+      </c>
+      <c r="I41" s="14">
+        <f t="shared" si="1"/>
+        <v>1092.6725019580474</v>
+      </c>
+      <c r="J41" s="14">
+        <v>5.16</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A42" s="15">
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
-      <c r="B42" s="16">
+      <c r="B42" s="14">
         <v>1.35</v>
       </c>
-      <c r="C42" s="17">
+      <c r="C42" s="15">
         <f>ROUND((C41*(B42^A42)), 0)</f>
         <v>40161787</v>
       </c>
-      <c r="D42" s="17">
+      <c r="D42" s="15">
         <f>ROUND((D41*(B42^A42)), 0)</f>
         <v>6477865</v>
       </c>
-      <c r="E42" s="17">
+      <c r="E42" s="15">
         <f>ROUND((E41*(B42^A42)), 0)</f>
         <v>24472</v>
       </c>
-      <c r="F42" s="17"/>
-      <c r="G42" s="17"/>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="17">
+      <c r="F42" s="15"/>
+      <c r="G42" s="16">
+        <f>G41/(H42^A41)</f>
+        <v>0.27621110153798156</v>
+      </c>
+      <c r="H42">
+        <v>1.0149999999999999</v>
+      </c>
+      <c r="I42" s="14">
+        <f t="shared" si="1"/>
+        <v>1980766.2693582645</v>
+      </c>
+      <c r="J42" s="14">
+        <v>1092.67</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A43" s="15">
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
-      <c r="B43" s="16">
+      <c r="B43" s="14">
         <v>1.35</v>
       </c>
-      <c r="C43" s="17">
+      <c r="C43" s="15">
         <f>ROUND((C42*(B43^A43)), 0)</f>
         <v>132685901008</v>
       </c>
-      <c r="D43" s="17">
+      <c r="D43" s="15">
         <f>ROUND((D42*(B43^A43)), 0)</f>
         <v>21401471855</v>
       </c>
-      <c r="E43" s="17">
+      <c r="E43" s="15">
         <f>ROUND((E42*(B43^A43)), 0)</f>
         <v>80850221</v>
       </c>
-      <c r="F43" s="17"/>
-      <c r="G43" s="17"/>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="17">
+      <c r="F43" s="15"/>
+      <c r="G43" s="16">
+        <f>G41/(H43^A42)</f>
+        <v>0.27212916407682919</v>
+      </c>
+      <c r="H43">
+        <v>1.0149999999999999</v>
+      </c>
+      <c r="I43" s="14">
+        <f t="shared" si="1"/>
+        <v>2674034.4636336574</v>
+      </c>
+      <c r="J43" s="14">
+        <v>1092.67</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A44" s="15">
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
-      <c r="B44" s="16">
+      <c r="B44" s="14">
         <v>1.35</v>
       </c>
-      <c r="C44" s="17">
+      <c r="C44" s="15">
         <f>ROUND((C42*(B44^A44)), 0)</f>
         <v>179125966361</v>
       </c>
-      <c r="D44" s="17">
+      <c r="D44" s="15">
         <f>ROUND((D42*(B44^A44)), 0)</f>
         <v>28891987005</v>
       </c>
-      <c r="E44" s="17">
+      <c r="E44" s="15">
         <f>ROUND((E42*(B44^A44)), 0)</f>
         <v>109147799</v>
       </c>
-      <c r="F44" s="17"/>
-      <c r="G44" s="17"/>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="17">
+      <c r="F44" s="15"/>
+      <c r="G44" s="16">
+        <f>G41/(H44^A43)</f>
+        <v>0.26810755081461007</v>
+      </c>
+      <c r="H44">
+        <v>1.0149999999999999</v>
+      </c>
+      <c r="I44" s="14">
+        <f t="shared" si="1"/>
+        <v>3609946.5259054373</v>
+      </c>
+      <c r="J44" s="14">
+        <v>1092.67</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A45" s="15">
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
-      <c r="B45" s="16">
+      <c r="B45" s="14">
         <v>1.35</v>
       </c>
-      <c r="C45" s="17">
+      <c r="C45" s="15">
         <f>ROUND((C42*(B45^A45)), 0)</f>
         <v>241820054588</v>
       </c>
-      <c r="D45" s="17">
+      <c r="D45" s="15">
         <f>ROUND((D42*(B45^A45)), 0)</f>
         <v>39004182456</v>
       </c>
-      <c r="E45" s="17">
+      <c r="E45" s="15">
         <f>ROUND((E42*(B45^A45)), 0)</f>
         <v>147349528</v>
       </c>
-      <c r="F45" s="17"/>
-      <c r="G45" s="17"/>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="17">
+      <c r="F45" s="15"/>
+      <c r="G45" s="16">
+        <f>G41/(H45^A44)</f>
+        <v>0.26414537026069962</v>
+      </c>
+      <c r="H45">
+        <v>1.0149999999999999</v>
+      </c>
+      <c r="I45" s="14">
+        <f t="shared" si="1"/>
+        <v>4873427.8099723402</v>
+      </c>
+      <c r="J45" s="14">
+        <v>1092.67</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A46" s="15">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="B46" s="16">
+      <c r="B46" s="14">
         <v>1.35</v>
       </c>
-      <c r="C46" s="17">
+      <c r="C46" s="15">
         <f>ROUND((C42*(B46^A46)), 0)</f>
         <v>326457073693</v>
       </c>
-      <c r="D46" s="17">
+      <c r="D46" s="15">
         <f>ROUND((D42*(B46^A46)), 0)</f>
         <v>52655646316</v>
       </c>
-      <c r="E46" s="17">
+      <c r="E46" s="15">
         <f>ROUND((E42*(B46^A46)), 0)</f>
         <v>198921863</v>
       </c>
-      <c r="F46" s="17"/>
-      <c r="G46" s="17"/>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="17">
+      <c r="F46" s="15"/>
+      <c r="G46" s="16">
+        <f>G41/(H46^A45)</f>
+        <v>0.26024174409921147</v>
+      </c>
+      <c r="H46">
+        <v>1.0149999999999999</v>
+      </c>
+      <c r="I46" s="14">
+        <f t="shared" si="1"/>
+        <v>6579127.543462662</v>
+      </c>
+      <c r="J46" s="14">
+        <v>1092.67</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A47" s="15">
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
-      <c r="B47" s="16">
+      <c r="B47" s="14">
         <v>1.35</v>
       </c>
-      <c r="C47" s="17">
+      <c r="C47" s="15">
         <f>ROUND((C42*(B47^A47)), 0)</f>
         <v>440717049486</v>
       </c>
-      <c r="D47" s="17">
+      <c r="D47" s="15">
         <f>ROUND((D42*(B47^A47)), 0)</f>
         <v>71085122526</v>
       </c>
-      <c r="E47" s="17">
+      <c r="E47" s="15">
         <f>ROUND((E42*(B47^A47)), 0)</f>
         <v>268544516</v>
       </c>
-      <c r="F47" s="17"/>
-      <c r="G47" s="17"/>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="17">
+      <c r="F47" s="15"/>
+      <c r="G47" s="16">
+        <f>G41/(H47^A46)</f>
+        <v>0.25639580699429709</v>
+      </c>
+      <c r="H47">
+        <v>1.0149999999999999</v>
+      </c>
+      <c r="I47" s="14">
+        <f t="shared" si="1"/>
+        <v>8881822.1836745944</v>
+      </c>
+      <c r="J47" s="14">
+        <v>1092.67</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A48" s="15">
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
-      <c r="B48" s="16">
+      <c r="B48" s="14">
         <v>1.35</v>
       </c>
-      <c r="C48" s="17">
+      <c r="C48" s="15">
         <f>ROUND((C42*(B48^A48)), 0)</f>
         <v>594968016806</v>
       </c>
-      <c r="D48" s="17">
+      <c r="D48" s="15">
         <f>ROUND((D42*(B48^A48)), 0)</f>
         <v>95964915410</v>
       </c>
-      <c r="E48" s="17">
+      <c r="E48" s="15">
         <f>ROUND((E42*(B48^A48)), 0)</f>
         <v>362535096</v>
       </c>
-      <c r="F48" s="17"/>
-      <c r="G48" s="17"/>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" s="17">
+      <c r="F48" s="15"/>
+      <c r="G48" s="16">
+        <f>G41/(H48^A47)</f>
+        <v>0.25260670639832228</v>
+      </c>
+      <c r="H48">
+        <v>1.0149999999999999</v>
+      </c>
+      <c r="I48" s="14">
+        <f t="shared" si="1"/>
+        <v>11990459.947960701</v>
+      </c>
+      <c r="J48" s="14">
+        <v>1092.67</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A49" s="15">
         <f t="shared" si="0"/>
         <v>33</v>
       </c>
-      <c r="B49" s="16">
+      <c r="B49" s="14">
         <v>1.35</v>
       </c>
-      <c r="C49" s="17">
+      <c r="C49" s="15">
         <f>ROUND((C42*(B49^A49)), 0)</f>
         <v>803206822689</v>
       </c>
-      <c r="D49" s="17">
+      <c r="D49" s="15">
         <f>ROUND((D42*(B49^A49)), 0)</f>
         <v>129552635804</v>
       </c>
-      <c r="E49" s="17">
+      <c r="E49" s="15">
         <f>ROUND((E42*(B49^A49)), 0)</f>
         <v>489422380</v>
       </c>
-      <c r="F49" s="17"/>
-      <c r="G49" s="17"/>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50" s="17">
+      <c r="F49" s="15"/>
+      <c r="G49" s="16">
+        <f>G41/(H49^A48)</f>
+        <v>0.24887360236287911</v>
+      </c>
+      <c r="H49">
+        <v>1.0149999999999999</v>
+      </c>
+      <c r="I49" s="14">
+        <f t="shared" si="1"/>
+        <v>16187120.929746946</v>
+      </c>
+      <c r="J49" s="14">
+        <v>1092.67</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A50" s="15">
         <f t="shared" si="0"/>
         <v>34</v>
       </c>
-      <c r="B50" s="16">
+      <c r="B50" s="14">
         <v>1.35</v>
       </c>
-      <c r="C50" s="17">
+      <c r="C50" s="15">
         <f>ROUND((C42*(B50^A50)), 0)</f>
         <v>1084329210629</v>
       </c>
-      <c r="D50" s="17">
+      <c r="D50" s="15">
         <f>ROUND((D42*(B50^A50)), 0)</f>
         <v>174896058336</v>
       </c>
-      <c r="E50" s="17">
+      <c r="E50" s="15">
         <f>ROUND((E42*(B50^A50)), 0)</f>
         <v>660720213</v>
       </c>
-      <c r="F50" s="17"/>
-      <c r="G50" s="17"/>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A51" s="17">
+      <c r="F50" s="15"/>
+      <c r="G50" s="16">
+        <f>G41/(H50^A49)</f>
+        <v>0.2451956673525903</v>
+      </c>
+      <c r="H50">
+        <v>1.0149999999999999</v>
+      </c>
+      <c r="I50" s="14">
+        <f t="shared" si="1"/>
+        <v>21852613.25515838</v>
+      </c>
+      <c r="J50" s="14">
+        <v>1092.67</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A51" s="15">
         <f t="shared" si="0"/>
         <v>35</v>
       </c>
-      <c r="B51" s="16">
+      <c r="B51" s="14">
         <v>1.35</v>
       </c>
-      <c r="C51" s="17">
+      <c r="C51" s="15">
         <f>ROUND((C42*(B51^A51)), 0)</f>
         <v>1463844434350</v>
       </c>
-      <c r="D51" s="17">
+      <c r="D51" s="15">
         <f>ROUND((D42*(B51^A51)), 0)</f>
         <v>236109678753</v>
       </c>
-      <c r="E51" s="17">
+      <c r="E51" s="15">
         <f>ROUND((E42*(B51^A51)), 0)</f>
         <v>891972287</v>
       </c>
-      <c r="F51" s="17">
+      <c r="F51" s="15">
         <v>10</v>
       </c>
-      <c r="G51" s="17"/>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A52" s="17">
+      <c r="G51" s="16">
+        <f>G41/(H51^A50)</f>
+        <v>0.24157208606166536</v>
+      </c>
+      <c r="H51">
+        <v>1.0149999999999999</v>
+      </c>
+      <c r="I51" s="14">
+        <f t="shared" si="1"/>
+        <v>29501027.894463811</v>
+      </c>
+      <c r="J51" s="14">
+        <v>1092.67</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A52" s="15">
         <f t="shared" si="0"/>
         <v>36</v>
       </c>
-      <c r="B52" s="16">
+      <c r="B52" s="14">
         <v>1.5</v>
       </c>
-      <c r="C52" s="17">
+      <c r="C52" s="15">
         <f>ROUND((C51*(B52^A52)), 0)</f>
         <v>3.1972769139291699E+18</v>
       </c>
-      <c r="D52" s="17">
+      <c r="D52" s="15">
         <f>ROUND((D51*(B52^A52)), 0)</f>
         <v>5.1570235697033299E+17</v>
       </c>
-      <c r="E52" s="17">
+      <c r="E52" s="15">
         <f>ROUND((E51*(B52^A52)), 0)</f>
         <v>1948214123146250</v>
       </c>
-      <c r="F52" s="17">
+      <c r="F52" s="15">
         <f>ROUND((F51*(B52^A52)), 0)</f>
         <v>21841644</v>
       </c>
-      <c r="G52" s="17"/>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A53" s="17">
+      <c r="G52" s="16">
+        <f>G51/(H52^A51)</f>
+        <v>0.15912148089394676</v>
+      </c>
+      <c r="H52">
+        <v>1.012</v>
+      </c>
+      <c r="I52" s="14">
+        <f t="shared" si="1"/>
+        <v>42956730098969.508</v>
+      </c>
+      <c r="J52" s="14">
+        <v>29501027.890000001</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A53" s="15">
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="B53" s="16">
+      <c r="B53" s="14">
         <v>1.5</v>
       </c>
-      <c r="C53" s="17">
+      <c r="C53" s="15">
         <f>ROUND((C51*(B53^A53)), 0)</f>
         <v>4.7959153708937503E+18</v>
       </c>
-      <c r="D53" s="17">
+      <c r="D53" s="15">
         <f>ROUND((D51*(B53^A53)), 0)</f>
         <v>7.7355353545549901E+17</v>
       </c>
-      <c r="E53" s="17">
+      <c r="E53" s="15">
         <f>ROUND((E51*(B53^A53)), 0)</f>
         <v>2922321184719370</v>
       </c>
-      <c r="F53" s="17">
+      <c r="F53" s="15">
         <f>ROUND((F51*(B53^A53)), 0)</f>
         <v>32762466</v>
       </c>
-      <c r="G53" s="17"/>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A54" s="17">
+      <c r="G53" s="16">
+        <f>G51/(H53^A52)</f>
+        <v>0.15723466491496715</v>
+      </c>
+      <c r="H53">
+        <v>1.012</v>
+      </c>
+      <c r="I53" s="14">
+        <f t="shared" si="1"/>
+        <v>64435095148454.273</v>
+      </c>
+      <c r="J53" s="14">
+        <v>29501027.890000001</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A54" s="15">
         <f t="shared" si="0"/>
         <v>38</v>
       </c>
-      <c r="B54" s="16">
+      <c r="B54" s="14">
         <v>1.5</v>
       </c>
-      <c r="C54" s="17">
+      <c r="C54" s="15">
         <f>ROUND((C51*(B54^A54)), 0)</f>
         <v>7.1938730563406203E+18</v>
       </c>
-      <c r="D54" s="17">
+      <c r="D54" s="15">
         <f>ROUND((D51*(B54^A54)), 0)</f>
         <v>1.1603303031832499E+18</v>
       </c>
-      <c r="E54" s="17">
+      <c r="E54" s="15">
         <f>ROUND((E51*(B54^A54)), 0)</f>
         <v>4383481777079060</v>
       </c>
-      <c r="F54" s="17">
+      <c r="F54" s="15">
         <f>ROUND((F51*(B54^A54)), 0)</f>
         <v>49143699</v>
       </c>
-      <c r="G54" s="17"/>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A55" s="17">
+      <c r="G54" s="16">
+        <f>G51/(H54^A53)</f>
+        <v>0.15537022224799127</v>
+      </c>
+      <c r="H54">
+        <v>1.012</v>
+      </c>
+      <c r="I54" s="14">
+        <f t="shared" si="1"/>
+        <v>96652642722681.406</v>
+      </c>
+      <c r="J54" s="14">
+        <v>29501027.890000001</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A55" s="15">
         <f t="shared" si="0"/>
         <v>39</v>
       </c>
-      <c r="B55" s="16">
+      <c r="B55" s="14">
         <v>1.5</v>
       </c>
-      <c r="C55" s="17">
+      <c r="C55" s="15">
         <f>ROUND((C51*(B55^A55)), 0)</f>
         <v>1.07908095845109E+19</v>
       </c>
-      <c r="D55" s="17">
+      <c r="D55" s="15">
         <f>ROUND((D51*(B55^A55)), 0)</f>
         <v>1.74049545477487E+18</v>
       </c>
-      <c r="E55" s="17">
+      <c r="E55" s="15">
         <f>ROUND((E51*(B55^A55)), 0)</f>
         <v>6575222665618590</v>
       </c>
-      <c r="F55" s="17">
+      <c r="F55" s="15">
         <f>ROUND((F51*(B55^A55)), 0)</f>
         <v>73715549</v>
       </c>
-      <c r="G55" s="17"/>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A56" s="17">
+      <c r="G55" s="16">
+        <f>G51/(H55^A54)</f>
+        <v>0.15352788759682934</v>
+      </c>
+      <c r="H55">
+        <v>1.012</v>
+      </c>
+      <c r="I55" s="14">
+        <f t="shared" si="1"/>
+        <v>144978964084022.09</v>
+      </c>
+      <c r="J55" s="14">
+        <v>29501027.890000001</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A56" s="15">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-      <c r="B56" s="16">
+      <c r="B56" s="14">
         <v>1.5</v>
       </c>
-      <c r="C56" s="17">
+      <c r="C56" s="15">
         <f>ROUND((C51*(B56^A56)), 0)</f>
         <v>1.6186214376766401E+19</v>
       </c>
-      <c r="D56" s="17">
+      <c r="D56" s="15">
         <f>ROUND((D51*(B56^A56)), 0)</f>
         <v>2.6107431821623101E+18</v>
       </c>
-      <c r="E56" s="17">
+      <c r="E56" s="15">
         <f>ROUND((E51*(B56^A56)), 0)</f>
         <v>9862833998427880</v>
       </c>
-      <c r="F56" s="17">
+      <c r="F56" s="15">
         <f>ROUND((F51*(B56^A56)), 0)</f>
         <v>110573323</v>
       </c>
-      <c r="G56" s="17"/>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A57" s="17">
+      <c r="G56" s="16">
+        <f>G51/(H56^A55)</f>
+        <v>0.15170739881109613</v>
+      </c>
+      <c r="H56">
+        <v>1.012</v>
+      </c>
+      <c r="I56" s="14">
+        <f t="shared" si="1"/>
+        <v>217468446126033.16</v>
+      </c>
+      <c r="J56" s="14">
+        <v>29501027.890000001</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A57" s="15">
         <f t="shared" si="0"/>
         <v>41</v>
       </c>
-      <c r="B57" s="16">
+      <c r="B57" s="14">
         <v>1.5</v>
       </c>
-      <c r="C57" s="17">
+      <c r="C57" s="15">
         <f>ROUND((C51*(B57^A57)), 0)</f>
         <v>2.4279321565149602E+19</v>
       </c>
-      <c r="D57" s="17">
+      <c r="D57" s="15">
         <f>ROUND((D51*(B57^A57)), 0)</f>
         <v>3.9161147732434698E+18</v>
       </c>
-      <c r="E57" s="17">
+      <c r="E57" s="15">
         <f>ROUND((E51*(B57^A57)), 0)</f>
         <v>1.47942509976418E+16</v>
       </c>
-      <c r="F57" s="17">
+      <c r="F57" s="15">
         <f>ROUND((F51*(B57^A57)), 0)</f>
         <v>165859985</v>
       </c>
-      <c r="G57" s="17"/>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A58" s="17">
+      <c r="G57" s="16">
+        <f>G51/(H57^A56)</f>
+        <v>0.14990849684890925</v>
+      </c>
+      <c r="H57">
+        <v>1.012</v>
+      </c>
+      <c r="I57" s="14">
+        <f t="shared" si="1"/>
+        <v>326202669189049.75</v>
+      </c>
+      <c r="J57" s="14">
+        <v>29501027.890000001</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A58" s="15">
         <f t="shared" si="0"/>
         <v>42</v>
       </c>
-      <c r="B58" s="16">
+      <c r="B58" s="14">
         <v>1.5</v>
       </c>
-      <c r="C58" s="17">
+      <c r="C58" s="15">
         <f>ROUND((C51*(B58^A58)), 0)</f>
         <v>3.6418982347724399E+19</v>
       </c>
-      <c r="D58" s="17">
+      <c r="D58" s="15">
         <f>ROUND((D51*(B58^A58)), 0)</f>
         <v>5.8741721598651996E+18</v>
       </c>
-      <c r="E58" s="17">
+      <c r="E58" s="15">
         <f>ROUND((E51*(B58^A58)), 0)</f>
         <v>2.21913764964627E+16</v>
       </c>
-      <c r="F58" s="17">
+      <c r="F58" s="15">
         <f>ROUND((F51*(B58^A58)), 0)</f>
         <v>248789977</v>
       </c>
-      <c r="G58" s="17"/>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A59" s="17">
+      <c r="G58" s="16">
+        <f>G51/(H58^A57)</f>
+        <v>0.1481309257400289</v>
+      </c>
+      <c r="H58">
+        <v>1.012</v>
+      </c>
+      <c r="I58" s="14">
+        <f t="shared" si="1"/>
+        <v>489304003783574.63</v>
+      </c>
+      <c r="J58" s="14">
+        <v>29501027.890000001</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A59" s="15">
         <f t="shared" si="0"/>
         <v>43</v>
       </c>
-      <c r="B59" s="16">
+      <c r="B59" s="14">
         <v>1.5</v>
       </c>
-      <c r="C59" s="17">
+      <c r="C59" s="15">
         <f>ROUND((C51*(B59^A59)), 0)</f>
         <v>5.4628473521586602E+19</v>
       </c>
-      <c r="D59" s="17">
+      <c r="D59" s="15">
         <f>ROUND((D51*(B59^A59)), 0)</f>
         <v>8.8112582397977999E+18</v>
       </c>
-      <c r="E59" s="17">
+      <c r="E59" s="15">
         <f>ROUND((E51*(B59^A59)), 0)</f>
         <v>3.32870647446941E+16</v>
       </c>
-      <c r="F59" s="17">
+      <c r="F59" s="15">
         <f>ROUND((F51*(B59^A59)), 0)</f>
         <v>373184966</v>
       </c>
-      <c r="G59" s="17"/>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A60" s="17">
+      <c r="G59" s="16">
+        <f>G51/(H59^A58)</f>
+        <v>0.14637443254943566</v>
+      </c>
+      <c r="H59">
+        <v>1.012</v>
+      </c>
+      <c r="I59" s="14">
+        <f t="shared" si="1"/>
+        <v>733956005675362</v>
+      </c>
+      <c r="J59" s="14">
+        <v>29501027.890000001</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A60" s="15">
         <f t="shared" si="0"/>
         <v>44</v>
       </c>
-      <c r="B60" s="16">
+      <c r="B60" s="14">
         <v>1.5</v>
       </c>
-      <c r="C60" s="17">
+      <c r="C60" s="15">
         <f>ROUND((C51*(B60^A60)), 0)</f>
         <v>8.1942710282379903E+19</v>
       </c>
-      <c r="D60" s="17">
+      <c r="D60" s="15">
         <f>ROUND((D51*(B60^A60)), 0)</f>
         <v>1.3216887359696699E+19</v>
       </c>
-      <c r="E60" s="17">
+      <c r="E60" s="15">
         <f>ROUND((E51*(B60^A60)), 0)</f>
         <v>4.9930597117041104E+16</v>
       </c>
-      <c r="F60" s="17">
+      <c r="F60" s="15">
         <f>ROUND((F51*(B60^A60)), 0)</f>
         <v>559777449</v>
       </c>
-      <c r="G60" s="17"/>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A61" s="17">
+      <c r="G60" s="16">
+        <f>G51/(H60^A59)</f>
+        <v>0.1446387673413396</v>
+      </c>
+      <c r="H60">
+        <v>1.012</v>
+      </c>
+      <c r="I60" s="14">
+        <f t="shared" si="1"/>
+        <v>1100934008513042.8</v>
+      </c>
+      <c r="J60" s="14">
+        <v>29501027.890000001</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A61" s="15">
         <f t="shared" si="0"/>
         <v>45</v>
       </c>
-      <c r="B61" s="16">
+      <c r="B61" s="14">
         <v>1.5</v>
       </c>
-      <c r="C61" s="17">
+      <c r="C61" s="15">
         <f>ROUND((C51*(B61^A61)), 0)</f>
         <v>1.2291406542356999E+20</v>
       </c>
-      <c r="D61" s="17">
+      <c r="D61" s="15">
         <f>ROUND((D51*(B61^A61)), 0)</f>
         <v>1.9825331039545E+19</v>
       </c>
-      <c r="E61" s="17">
+      <c r="E61" s="15">
         <f>ROUND((E51*(B61^A61)), 0)</f>
         <v>7.4895895675561696E+16</v>
       </c>
-      <c r="F61" s="17">
+      <c r="F61" s="15">
         <f>ROUND((F51*(B61^A61)), 0)</f>
         <v>839666173</v>
       </c>
-      <c r="G61" s="17"/>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A62" s="17">
+      <c r="G61" s="16">
+        <f>G51/(H61^A60)</f>
+        <v>0.14292368314361623</v>
+      </c>
+      <c r="H61">
+        <v>1.012</v>
+      </c>
+      <c r="I61" s="14">
+        <f t="shared" si="1"/>
+        <v>1651401012769564.3</v>
+      </c>
+      <c r="J61" s="14">
+        <v>29501027.890000001</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A62" s="15">
         <f t="shared" si="0"/>
         <v>46</v>
       </c>
-      <c r="B62" s="16">
+      <c r="B62" s="14">
         <v>1.5</v>
       </c>
-      <c r="C62" s="17">
+      <c r="C62" s="15">
         <f>ROUND((C51*(B62^A62)), 0)</f>
         <v>1.84371098135355E+20</v>
       </c>
-      <c r="D62" s="17">
+      <c r="D62" s="15">
         <f>ROUND((D51*(B62^A62)), 0)</f>
         <v>2.9737996559317598E+19</v>
       </c>
-      <c r="E62" s="17">
+      <c r="E62" s="15">
         <f>ROUND((E51*(B62^A62)), 0)</f>
         <v>1.1234384351334301E+17</v>
       </c>
-      <c r="F62" s="17">
+      <c r="F62" s="15">
         <f>ROUND((F51*(B62^A62)), 0)</f>
         <v>1259499260</v>
       </c>
-      <c r="G62" s="17"/>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A63" s="17">
+      <c r="G62" s="16">
+        <f>G51/(H62^A61)</f>
+        <v>0.14122893591266425</v>
+      </c>
+      <c r="H62">
+        <v>1.012</v>
+      </c>
+      <c r="I62" s="14">
+        <f t="shared" si="1"/>
+        <v>2477101519154346.5</v>
+      </c>
+      <c r="J62" s="14">
+        <v>29501027.890000001</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A63" s="15">
         <f t="shared" si="0"/>
         <v>47</v>
       </c>
-      <c r="B63" s="16">
+      <c r="B63" s="14">
         <v>1.5</v>
       </c>
-      <c r="C63" s="17">
+      <c r="C63" s="15">
         <f>ROUND((C51*(B63^A63)), 0)</f>
         <v>2.7655664720303201E+20</v>
       </c>
-      <c r="D63" s="17">
+      <c r="D63" s="15">
         <f>ROUND((D51*(B63^A63)), 0)</f>
         <v>4.4606994838976299E+19</v>
       </c>
-      <c r="E63" s="17">
+      <c r="E63" s="15">
         <f>ROUND((E51*(B63^A63)), 0)</f>
         <v>1.6851576527001402E+17</v>
       </c>
-      <c r="F63" s="17">
+      <c r="F63" s="15">
         <f>ROUND((F51*(B63^A63)), 0)</f>
         <v>1889248890</v>
       </c>
-      <c r="G63" s="17"/>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A64" s="17">
+      <c r="G63" s="16">
+        <f>G51/(H63^A62)</f>
+        <v>0.1395542844986801</v>
+      </c>
+      <c r="H63">
+        <v>1.012</v>
+      </c>
+      <c r="I63" s="14">
+        <f t="shared" si="1"/>
+        <v>3715652278731520</v>
+      </c>
+      <c r="J63" s="14">
+        <v>29501027.890000001</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A64" s="15">
         <f t="shared" si="0"/>
         <v>48</v>
       </c>
-      <c r="B64" s="16">
+      <c r="B64" s="14">
         <v>1.5</v>
       </c>
-      <c r="C64" s="17">
+      <c r="C64" s="15">
         <f>ROUND((C51*(B64^A64)), 0)</f>
         <v>4.1483497080454801E+20</v>
       </c>
-      <c r="D64" s="17">
+      <c r="D64" s="15">
         <f>ROUND((D51*(B64^A64)), 0)</f>
         <v>6.6910492258464498E+19</v>
       </c>
-      <c r="E64" s="17">
+      <c r="E64" s="15">
         <f>ROUND((E51*(B64^A64)), 0)</f>
         <v>2.5277364790502099E+17</v>
       </c>
-      <c r="F64" s="17">
+      <c r="F64" s="15">
         <f>ROUND((F51*(B64^A64)), 0)</f>
         <v>2833873334</v>
       </c>
-      <c r="G64" s="17"/>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A65" s="17">
+      <c r="G64" s="16">
+        <f>G51/(H64^A63)</f>
+        <v>0.13789949061134393</v>
+      </c>
+      <c r="H64">
+        <v>1.012</v>
+      </c>
+      <c r="I64" s="14">
+        <f t="shared" si="1"/>
+        <v>5573478418097279</v>
+      </c>
+      <c r="J64" s="14">
+        <v>29501027.890000001</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A65" s="15">
         <f t="shared" si="0"/>
         <v>49</v>
       </c>
-      <c r="B65" s="16">
+      <c r="B65" s="14">
         <v>1.5</v>
       </c>
-      <c r="C65" s="17">
+      <c r="C65" s="15">
         <f>ROUND((C51*(B65^A65)), 0)</f>
         <v>6.2225245620682306E+20</v>
       </c>
-      <c r="D65" s="17">
+      <c r="D65" s="15">
         <f>ROUND((D51*(B65^A65)), 0)</f>
         <v>1.0036573838769699E+20</v>
       </c>
-      <c r="E65" s="17">
+      <c r="E65" s="15">
         <f>ROUND((E51*(B65^A65)), 0)</f>
         <v>3.7916047185753101E+17</v>
       </c>
-      <c r="F65" s="17">
+      <c r="F65" s="15">
         <f>ROUND((F51*(B65^A65)), 0)</f>
         <v>4250810001</v>
       </c>
-      <c r="G65" s="17"/>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A66" s="17">
+      <c r="G65" s="16">
+        <f>G51/(H65^A64)</f>
+        <v>0.13626431878591297</v>
+      </c>
+      <c r="H65">
+        <v>1.012</v>
+      </c>
+      <c r="I65" s="14">
+        <f t="shared" si="1"/>
+        <v>8360217627145920</v>
+      </c>
+      <c r="J65" s="14">
+        <v>29501027.890000001</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A66" s="15">
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
-      <c r="B66" s="16">
+      <c r="B66" s="14">
         <v>1.5</v>
       </c>
-      <c r="C66" s="17">
+      <c r="C66" s="15">
         <f>ROUND((C51*(B66^A66)), 0)</f>
         <v>9.3337868431023394E+20</v>
       </c>
-      <c r="D66" s="17">
+      <c r="D66" s="15">
         <f>ROUND((D51*(B66^A66)), 0)</f>
         <v>1.5054860758154501E+20</v>
       </c>
-      <c r="E66" s="17">
+      <c r="E66" s="15">
         <f>ROUND((E51*(B66^A66)), 0)</f>
         <v>5.6874070778629702E+17</v>
       </c>
-      <c r="F66" s="17">
+      <c r="F66" s="15">
         <f>ROUND((F51*(B66^A66)), 0)</f>
         <v>6376215002</v>
       </c>
-      <c r="G66" s="17"/>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A67" s="17">
+      <c r="G66" s="16">
+        <f>G51/(H66^A65)</f>
+        <v>0.13464853634971638</v>
+      </c>
+      <c r="H66">
+        <v>1.012</v>
+      </c>
+      <c r="I66" s="14">
+        <f t="shared" si="1"/>
+        <v>1.2540326440718878E+16</v>
+      </c>
+      <c r="J66" s="14">
+        <v>29501027.890000001</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A67" s="15">
         <f t="shared" si="0"/>
         <v>51</v>
       </c>
-      <c r="B67" s="16">
+      <c r="B67" s="14">
         <v>1.3</v>
       </c>
-      <c r="C67" s="17">
+      <c r="C67" s="15">
         <f>ROUND((C66*(B67^A67)), 0)</f>
         <v>6.0418347993103903E+26</v>
       </c>
-      <c r="D67" s="17">
+      <c r="D67" s="15">
         <f>ROUND((D66*(B67^A67)), 0)</f>
         <v>9.74513165517689E+25</v>
       </c>
-      <c r="E67" s="17">
+      <c r="E67" s="15">
         <f>ROUND((E66*(B67^A67)), 0)</f>
         <v>3.68150404316019E+23</v>
       </c>
-      <c r="F67" s="17">
+      <c r="F67" s="15">
         <f>ROUND((F66*(B67^A67)), 0)</f>
         <v>4127374915941840</v>
       </c>
-      <c r="G67" s="17"/>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A68" s="17">
+      <c r="G67" s="16">
+        <f>G66/(H67^A66)</f>
+        <v>8.1871537788168802E-2</v>
+      </c>
+      <c r="H67">
+        <v>1.01</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A68" s="15">
         <f t="shared" si="0"/>
         <v>52</v>
       </c>
-      <c r="B68" s="16">
+      <c r="B68" s="14">
         <v>1.3</v>
       </c>
-      <c r="C68" s="17">
+      <c r="C68" s="15">
         <f>ROUND((C66*(B68^A68)), 0)</f>
         <v>7.8543852391035001E+26</v>
       </c>
-      <c r="D68" s="17">
+      <c r="D68" s="15">
         <f>ROUND((D66*(B68^A68)), 0)</f>
         <v>1.2668671151729999E+26</v>
       </c>
-      <c r="E68" s="17">
+      <c r="E68" s="15">
         <f>ROUND((E66*(B68^A68)), 0)</f>
         <v>4.7859552561082503E+23</v>
       </c>
-      <c r="F68" s="17">
+      <c r="F68" s="15">
         <f>ROUND((F66*(B68^A68)), 0)</f>
         <v>5365587390724390</v>
       </c>
-      <c r="G68" s="17"/>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A69" s="17">
+      <c r="G68" s="16">
+        <f>G66/(H68^A67)</f>
+        <v>8.1060928503137453E-2</v>
+      </c>
+      <c r="H68">
+        <v>1.01</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A69" s="15">
         <f t="shared" si="0"/>
         <v>53</v>
       </c>
-      <c r="B69" s="16">
+      <c r="B69" s="14">
         <v>1.3</v>
       </c>
-      <c r="C69" s="17">
+      <c r="C69" s="15">
         <f>ROUND((C66*(B69^A69)), 0)</f>
         <v>1.02107008108346E+27</v>
       </c>
-      <c r="D69" s="17">
+      <c r="D69" s="15">
         <f>ROUND((D66*(B69^A69)), 0)</f>
         <v>1.6469272497248901E+26</v>
       </c>
-      <c r="E69" s="17">
+      <c r="E69" s="15">
         <f>ROUND((E66*(B69^A69)), 0)</f>
         <v>6.2217418329407304E+23</v>
       </c>
-      <c r="F69" s="17">
+      <c r="F69" s="15">
         <f>ROUND((F66*(B69^A69)), 0)</f>
         <v>6975263607941700</v>
       </c>
-      <c r="G69" s="17"/>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A70" s="17">
+      <c r="G69" s="16">
+        <f>G66/(H69^A68)</f>
+        <v>8.0258345052611327E-2</v>
+      </c>
+      <c r="H69">
+        <v>1.01</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A70" s="15">
         <f t="shared" si="0"/>
         <v>54</v>
       </c>
-      <c r="B70" s="16">
+      <c r="B70" s="14">
         <v>1.3</v>
       </c>
-      <c r="C70" s="17">
+      <c r="C70" s="15">
         <f>ROUND((C66*(B70^A70)), 0)</f>
         <v>1.3273911054084901E+27</v>
       </c>
-      <c r="D70" s="17">
+      <c r="D70" s="15">
         <f>ROUND((D66*(B70^A70)), 0)</f>
         <v>2.1410054246423599E+26</v>
       </c>
-      <c r="E70" s="17">
+      <c r="E70" s="15">
         <f>ROUND((E66*(B70^A70)), 0)</f>
         <v>8.0882643828229496E+23</v>
       </c>
-      <c r="F70" s="17">
+      <c r="F70" s="15">
         <f>ROUND((F66*(B70^A70)), 0)</f>
         <v>9067842690324220</v>
       </c>
-      <c r="G70" s="17"/>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A71" s="17">
+      <c r="G70" s="16">
+        <f>G66/(H70^A69)</f>
+        <v>7.9463707972882519E-2</v>
+      </c>
+      <c r="H70">
+        <v>1.01</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A71" s="15">
         <f t="shared" si="0"/>
         <v>55</v>
       </c>
-      <c r="B71" s="16">
+      <c r="B71" s="14">
         <v>1.3</v>
       </c>
-      <c r="C71" s="17">
+      <c r="C71" s="15">
         <f>ROUND((C66*(B71^A71)), 0)</f>
         <v>1.72560843703104E+27</v>
       </c>
-      <c r="D71" s="17">
+      <c r="D71" s="15">
         <f>ROUND((D66*(B71^A71)), 0)</f>
         <v>2.78330705203507E+26</v>
       </c>
-      <c r="E71" s="17">
+      <c r="E71" s="15">
         <f>ROUND((E66*(B71^A71)), 0)</f>
         <v>1.05147436976698E+24</v>
       </c>
-      <c r="F71" s="17">
+      <c r="F71" s="15">
         <f>ROUND((F66*(B71^A71)), 0)</f>
         <v>1.17881954974215E+16</v>
       </c>
-      <c r="G71" s="17"/>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A72" s="17">
+      <c r="G71" s="16">
+        <f>G66/(H71^A70)</f>
+        <v>7.8676938587012371E-2</v>
+      </c>
+      <c r="H71">
+        <v>1.01</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A72" s="15">
         <f t="shared" si="0"/>
         <v>56</v>
       </c>
-      <c r="B72" s="16">
+      <c r="B72" s="14">
         <v>1.3</v>
       </c>
-      <c r="C72" s="17">
+      <c r="C72" s="15">
         <f>ROUND((C66*(B72^A72)), 0)</f>
         <v>2.2432909681403499E+27</v>
       </c>
-      <c r="D72" s="17">
+      <c r="D72" s="15">
         <f>ROUND((D66*(B72^A72)), 0)</f>
         <v>3.6182991676455903E+26</v>
       </c>
-      <c r="E72" s="17">
+      <c r="E72" s="15">
         <f>ROUND((E66*(B72^A72)), 0)</f>
         <v>1.36691668069708E+24</v>
       </c>
-      <c r="F72" s="17">
+      <c r="F72" s="15">
         <f>ROUND((F66*(B72^A72)), 0)</f>
         <v>1.53246541466479E+16</v>
       </c>
-      <c r="G72" s="17"/>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A73" s="17">
+      <c r="G72" s="16">
+        <f>G66/(H72^A71)</f>
+        <v>7.7897958997041966E-2</v>
+      </c>
+      <c r="H72">
+        <v>1.01</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A73" s="15">
         <f t="shared" si="0"/>
         <v>57</v>
       </c>
-      <c r="B73" s="16">
+      <c r="B73" s="14">
         <v>1.3</v>
       </c>
-      <c r="C73" s="17">
+      <c r="C73" s="15">
         <f>ROUND((C66*(B73^A73)), 0)</f>
         <v>2.91627825858246E+27</v>
       </c>
-      <c r="D73" s="17">
+      <c r="D73" s="15">
         <f>ROUND((D66*(B73^A73)), 0)</f>
         <v>4.7037889179392701E+26</v>
       </c>
-      <c r="E73" s="17">
+      <c r="E73" s="15">
         <f>ROUND((E66*(B73^A73)), 0)</f>
         <v>1.7769916849061999E+24</v>
       </c>
-      <c r="F73" s="17">
+      <c r="F73" s="15">
         <f>ROUND((F66*(B73^A73)), 0)</f>
         <v>1.99220503906423E+16</v>
       </c>
-      <c r="G73" s="17"/>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A74" s="17">
+      <c r="G73" s="16">
+        <f>G66/(H73^A72)</f>
+        <v>7.712669207627916E-2</v>
+      </c>
+      <c r="H73">
+        <v>1.01</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A74" s="15">
         <f t="shared" si="0"/>
         <v>58</v>
       </c>
-      <c r="B74" s="16">
+      <c r="B74" s="14">
         <v>1.3</v>
       </c>
-      <c r="C74" s="17">
+      <c r="C74" s="15">
         <f>ROUND((C66*(B74^A74)), 0)</f>
         <v>3.7911617361571901E+27</v>
       </c>
-      <c r="D74" s="17">
+      <c r="D74" s="15">
         <f>ROUND((D66*(B74^A74)), 0)</f>
         <v>6.1149255933210497E+26</v>
       </c>
-      <c r="E74" s="17">
+      <c r="E74" s="15">
         <f>ROUND((E66*(B74^A74)), 0)</f>
         <v>2.3100891903780601E+24</v>
       </c>
-      <c r="F74" s="17">
+      <c r="F74" s="15">
         <f>ROUND((F66*(B74^A74)), 0)</f>
         <v>2.5898665507835E+16</v>
       </c>
-      <c r="G74" s="17"/>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A75" s="17">
+      <c r="G74" s="16">
+        <f>G66/(H74^A73)</f>
+        <v>7.6363061461662524E-2</v>
+      </c>
+      <c r="H74">
+        <v>1.01</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A75" s="15">
         <f t="shared" si="0"/>
         <v>59</v>
       </c>
-      <c r="B75" s="16">
+      <c r="B75" s="14">
         <v>1.3</v>
       </c>
-      <c r="C75" s="17">
+      <c r="C75" s="15">
         <f>ROUND((C66*(B75^A75)), 0)</f>
         <v>4.9285102570043498E+27</v>
       </c>
-      <c r="D75" s="17">
+      <c r="D75" s="15">
         <f>ROUND((D66*(B75^A75)), 0)</f>
         <v>7.9494032713173697E+26</v>
       </c>
-      <c r="E75" s="17">
+      <c r="E75" s="15">
         <f>ROUND((E66*(B75^A75)), 0)</f>
         <v>3.0031159474914802E+24</v>
       </c>
-      <c r="F75" s="17">
+      <c r="F75" s="15">
         <f>ROUND((F66*(B75^A75)), 0)</f>
         <v>3.36682651601855E+16</v>
       </c>
-      <c r="G75" s="17"/>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A76" s="17">
+      <c r="G75" s="16">
+        <f>G66/(H75^A74)</f>
+        <v>7.5606991546200514E-2</v>
+      </c>
+      <c r="H75">
+        <v>1.01</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A76" s="15">
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
-      <c r="B76" s="16">
+      <c r="B76" s="14">
         <v>1.3</v>
       </c>
-      <c r="C76" s="17">
+      <c r="C76" s="15">
         <f>ROUND((C66*(B76^A76)), 0)</f>
         <v>6.4070633341056605E+27</v>
       </c>
-      <c r="D76" s="17">
+      <c r="D76" s="15">
         <f>ROUND((D66*(B76^A76)), 0)</f>
         <v>1.03342242527126E+27</v>
       </c>
-      <c r="E76" s="17">
+      <c r="E76" s="15">
         <f>ROUND((E66*(B76^A76)), 0)</f>
         <v>3.9040507317389299E+24</v>
       </c>
-      <c r="F76" s="17">
+      <c r="F76" s="15">
         <f>ROUND((F66*(B76^A76)), 0)</f>
         <v>4.3768744708241104E+16</v>
       </c>
-      <c r="G76" s="17"/>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A77" s="17">
+      <c r="G76" s="16">
+        <f>G66/(H76^A75)</f>
+        <v>7.4858407471485686E-2</v>
+      </c>
+      <c r="H76">
+        <v>1.01</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A77" s="15">
         <f t="shared" si="0"/>
         <v>61</v>
       </c>
-      <c r="B77" s="16">
+      <c r="B77" s="14">
         <v>1.3</v>
       </c>
-      <c r="C77" s="17">
+      <c r="C77" s="15">
         <f>ROUND((C66*(B77^A77)), 0)</f>
         <v>8.3291823343373595E+27</v>
       </c>
-      <c r="D77" s="17">
+      <c r="D77" s="15">
         <f>ROUND((D66*(B77^A77)), 0)</f>
         <v>1.3434491528526401E+27</v>
       </c>
-      <c r="E77" s="17">
+      <c r="E77" s="15">
         <f>ROUND((E66*(B77^A77)), 0)</f>
         <v>5.0752659512606003E+24</v>
       </c>
-      <c r="F77" s="17">
+      <c r="F77" s="15">
         <f>ROUND((F66*(B77^A77)), 0)</f>
         <v>5.6899368120713504E+16</v>
       </c>
-      <c r="G77" s="17"/>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A78" s="17">
+      <c r="G77" s="16">
+        <f>G66/(H77^A76)</f>
+        <v>7.4117235120282857E-2</v>
+      </c>
+      <c r="H77">
+        <v>1.01</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A78" s="15">
         <f t="shared" si="0"/>
         <v>62</v>
       </c>
-      <c r="B78" s="16">
+      <c r="B78" s="14">
         <v>1.3</v>
       </c>
-      <c r="C78" s="17">
+      <c r="C78" s="15">
         <f>ROUND((C66*(B78^A78)), 0)</f>
         <v>1.08279370346386E+28</v>
       </c>
-      <c r="D78" s="17">
+      <c r="D78" s="15">
         <f>ROUND((D66*(B78^A78)), 0)</f>
         <v>1.7464838987084299E+27</v>
       </c>
-      <c r="E78" s="17">
+      <c r="E78" s="15">
         <f>ROUND((E66*(B78^A78)), 0)</f>
         <v>6.59784573663878E+24</v>
       </c>
-      <c r="F78" s="17">
+      <c r="F78" s="15">
         <f>ROUND((F66*(B78^A78)), 0)</f>
         <v>7.39691785569276E+16</v>
       </c>
-      <c r="G78" s="17"/>
-    </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A79" s="17">
+      <c r="G78" s="16">
+        <f>G66/(H78^A77)</f>
+        <v>7.3383401109190935E-2</v>
+      </c>
+      <c r="H78">
+        <v>1.01</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A79" s="15">
         <f t="shared" si="0"/>
         <v>63</v>
       </c>
-      <c r="B79" s="16">
+      <c r="B79" s="14">
         <v>1.3</v>
       </c>
-      <c r="C79" s="17">
+      <c r="C79" s="15">
         <f>ROUND((C66*(B79^A79)), 0)</f>
         <v>1.4076318145030101E+28</v>
       </c>
-      <c r="D79" s="17">
+      <c r="D79" s="15">
         <f>ROUND((D66*(B79^A79)), 0)</f>
         <v>2.27042906832095E+27</v>
       </c>
-      <c r="E79" s="17">
+      <c r="E79" s="15">
         <f>ROUND((E66*(B79^A79)), 0)</f>
         <v>8.5771994576304203E+24</v>
       </c>
-      <c r="F79" s="17">
+      <c r="F79" s="15">
         <f>ROUND((F66*(B79^A79)), 0)</f>
         <v>9.6159932124005792E+16</v>
       </c>
-      <c r="G79" s="17"/>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A80" s="17">
+      <c r="G79" s="16">
+        <f>G66/(H79^A78)</f>
+        <v>7.2656832781377148E-2</v>
+      </c>
+      <c r="H79">
+        <v>1.01</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A80" s="15">
         <f t="shared" si="0"/>
         <v>64</v>
       </c>
-      <c r="B80" s="16">
+      <c r="B80" s="14">
         <v>1.3</v>
       </c>
-      <c r="C80" s="17">
+      <c r="C80" s="15">
         <f>ROUND((C66*(B80^A80)), 0)</f>
         <v>1.82992135885392E+28</v>
       </c>
-      <c r="D80" s="17">
+      <c r="D80" s="15">
         <f>ROUND((D66*(B80^A80)), 0)</f>
         <v>2.9515577888172398E+27</v>
       </c>
-      <c r="E80" s="17">
+      <c r="E80" s="15">
         <f>ROUND((E66*(B80^A80)), 0)</f>
         <v>1.11503592949195E+25</v>
       </c>
-      <c r="F80" s="17">
+      <c r="F80" s="15">
         <f>ROUND((F66*(B80^A80)), 0)</f>
         <v>1.25007911761208E+17</v>
       </c>
-      <c r="G80" s="17"/>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A81" s="17">
+      <c r="G80" s="16">
+        <f>G66/(H80^A79)</f>
+        <v>7.1937458199383339E-2</v>
+      </c>
+      <c r="H80">
+        <v>1.01</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A81" s="15">
         <f t="shared" si="0"/>
         <v>65</v>
       </c>
-      <c r="B81" s="16">
+      <c r="B81" s="14">
         <v>1.3</v>
       </c>
-      <c r="C81" s="17">
+      <c r="C81" s="15">
         <f>ROUND((C66*(B81^A81)), 0)</f>
         <v>2.3788977665100898E+28</v>
       </c>
-      <c r="D81" s="17">
+      <c r="D81" s="15">
         <f>ROUND((D66*(B81^A81)), 0)</f>
         <v>3.8370251254624098E+27</v>
       </c>
-      <c r="E81" s="17">
+      <c r="E81" s="15">
         <f>ROUND((E66*(B81^A81)), 0)</f>
         <v>1.4495467083395401E+25</v>
       </c>
-      <c r="F81" s="17">
+      <c r="F81" s="15">
         <f>ROUND((F66*(B81^A81)), 0)</f>
         <v>1.6251028528956998E+17</v>
       </c>
-      <c r="G81" s="17"/>
-    </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A82" s="17">
+      <c r="G81" s="16">
+        <f>G66/(H81^A80)</f>
+        <v>7.1225206138003289E-2</v>
+      </c>
+      <c r="H81">
+        <v>1.01</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A82" s="15">
         <f t="shared" si="0"/>
         <v>66</v>
       </c>
-      <c r="B82" s="16">
+      <c r="B82" s="14">
         <v>1.17</v>
       </c>
-      <c r="C82" s="17">
+      <c r="C82" s="15">
         <f>ROUND((C81*(B82^A82)), 0)</f>
         <v>7.52735942661637E+32</v>
       </c>
-      <c r="D82" s="17">
+      <c r="D82" s="15">
         <f>ROUND((D81*(B82^A82)), 0)</f>
         <v>1.2141197345645101E+32</v>
       </c>
-      <c r="E82" s="17">
+      <c r="E82" s="15">
         <f>ROUND((E81*(B82^A82)), 0)</f>
         <v>4.5866868399929098E+29</v>
       </c>
-      <c r="F82" s="17">
+      <c r="F82" s="15">
         <f>ROUND((F81*(B82^A82)), 0)</f>
         <v>5.1421853646579198E+21</v>
       </c>
-      <c r="G82" s="17"/>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A83" s="17">
-        <f t="shared" ref="A83:A128" si="1">A82+1</f>
+      <c r="G82" s="16">
+        <f>G81/(H82^A81)</f>
+        <v>4.8279745048010241E-2</v>
+      </c>
+      <c r="H82">
+        <v>1.006</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A83" s="15">
+        <f t="shared" ref="A83:A116" si="2">A82+1</f>
         <v>67</v>
       </c>
-      <c r="B83" s="16">
+      <c r="B83" s="14">
         <v>1.17</v>
       </c>
-      <c r="C83" s="17">
+      <c r="C83" s="15">
         <f>ROUND((C81*(B83^A83)), 0)</f>
         <v>8.8070105291411501E+32</v>
       </c>
-      <c r="D83" s="17">
+      <c r="D83" s="15">
         <f>ROUND((D81*(B83^A83)), 0)</f>
         <v>1.4205200894404699E+32</v>
       </c>
-      <c r="E83" s="17">
+      <c r="E83" s="15">
         <f>ROUND((E81*(B83^A83)), 0)</f>
         <v>5.3664236027917102E+29</v>
       </c>
-      <c r="F83" s="17">
+      <c r="F83" s="15">
         <f>ROUND((F81*(B83^A83)), 0)</f>
         <v>6.0163568766497703E+21</v>
       </c>
-      <c r="G83" s="17"/>
-    </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A84" s="17">
-        <f t="shared" si="1"/>
+      <c r="G83" s="16">
+        <f>G81/(H83^A82)</f>
+        <v>4.7991794282316341E-2</v>
+      </c>
+      <c r="H83">
+        <v>1.006</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A84" s="15">
+        <f t="shared" si="2"/>
         <v>68</v>
       </c>
-      <c r="B84" s="16">
+      <c r="B84" s="14">
         <v>1.17</v>
       </c>
-      <c r="C84" s="17">
+      <c r="C84" s="15">
         <f>ROUND((C81*(B84^A84)), 0)</f>
         <v>1.0304202319095099E+33</v>
       </c>
-      <c r="D84" s="17">
+      <c r="D84" s="15">
         <f>ROUND((D81*(B84^A84)), 0)</f>
         <v>1.6620085046453601E+32</v>
       </c>
-      <c r="E84" s="17">
+      <c r="E84" s="15">
         <f>ROUND((E81*(B84^A84)), 0)</f>
         <v>6.2787156152663001E+29</v>
       </c>
-      <c r="F84" s="17">
+      <c r="F84" s="15">
         <f>ROUND((F81*(B84^A84)), 0)</f>
         <v>7.0391375456802303E+21</v>
       </c>
-      <c r="G84" s="17"/>
-    </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A85" s="17">
-        <f t="shared" si="1"/>
+      <c r="G84" s="16">
+        <f>G81/(H84^A83)</f>
+        <v>4.7705560916815451E-2</v>
+      </c>
+      <c r="H84">
+        <v>1.006</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A85" s="15">
+        <f t="shared" si="2"/>
         <v>69</v>
       </c>
-      <c r="B85" s="16">
+      <c r="B85" s="14">
         <v>1.17</v>
       </c>
-      <c r="C85" s="17">
+      <c r="C85" s="15">
         <f>ROUND((C81*(B85^A85)), 0)</f>
         <v>1.2055916713341301E+33</v>
       </c>
-      <c r="D85" s="17">
+      <c r="D85" s="15">
         <f>ROUND((D81*(B85^A85)), 0)</f>
         <v>1.94454995043507E+32</v>
       </c>
-      <c r="E85" s="17">
+      <c r="E85" s="15">
         <f>ROUND((E81*(B85^A85)), 0)</f>
         <v>7.3460972698615701E+29</v>
       </c>
-      <c r="F85" s="17">
+      <c r="F85" s="15">
         <f>ROUND((F81*(B85^A85)), 0)</f>
         <v>8.2357909284458605E+21</v>
       </c>
-      <c r="G85" s="17"/>
-    </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A86" s="17">
-        <f t="shared" si="1"/>
+      <c r="G85" s="16">
+        <f>G81/(H85^A84)</f>
+        <v>4.7421034708564055E-2</v>
+      </c>
+      <c r="H85">
+        <v>1.006</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A86" s="15">
+        <f t="shared" si="2"/>
         <v>70</v>
       </c>
-      <c r="B86" s="16">
+      <c r="B86" s="14">
         <v>1.17</v>
       </c>
-      <c r="C86" s="17">
+      <c r="C86" s="15">
         <f>ROUND((C81*(B86^A86)), 0)</f>
         <v>1.4105422554609301E+33</v>
       </c>
-      <c r="D86" s="17">
+      <c r="D86" s="15">
         <f>ROUND((D81*(B86^A86)), 0)</f>
         <v>2.2751234420090302E+32</v>
       </c>
-      <c r="E86" s="17">
+      <c r="E86" s="15">
         <f>ROUND((E81*(B86^A86)), 0)</f>
         <v>8.5949338057380394E+29</v>
       </c>
-      <c r="F86" s="17">
+      <c r="F86" s="15">
         <f>ROUND((F81*(B86^A86)), 0)</f>
         <v>9.6358753862816597E+21</v>
       </c>
-      <c r="G86" s="17"/>
-    </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A87" s="17">
-        <f t="shared" si="1"/>
+      <c r="G86" s="16">
+        <f>G81/(H86^A85)</f>
+        <v>4.71382054757098E-2</v>
+      </c>
+      <c r="H86">
+        <v>1.006</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A87" s="15">
+        <f t="shared" si="2"/>
         <v>71</v>
       </c>
-      <c r="B87" s="16">
+      <c r="B87" s="14">
         <v>1.17</v>
       </c>
-      <c r="C87" s="17">
+      <c r="C87" s="15">
         <f>ROUND((C81*(B87^A87)), 0)</f>
         <v>1.6503344388892899E+33</v>
       </c>
-      <c r="D87" s="17">
+      <c r="D87" s="15">
         <f>ROUND((D81*(B87^A87)), 0)</f>
         <v>2.6618944271505601E+32</v>
       </c>
-      <c r="E87" s="17">
+      <c r="E87" s="15">
         <f>ROUND((E81*(B87^A87)), 0)</f>
         <v>1.0056072552713501E+30</v>
       </c>
-      <c r="F87" s="17">
+      <c r="F87" s="15">
         <f>ROUND((F81*(B87^A87)), 0)</f>
         <v>1.1273974201949501E+22</v>
       </c>
-      <c r="G87" s="17"/>
-    </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A88" s="17">
-        <f t="shared" si="1"/>
+      <c r="G87" s="16">
+        <f>G81/(H87^A86)</f>
+        <v>4.685706309712704E-2</v>
+      </c>
+      <c r="H87">
+        <v>1.006</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A88" s="15">
+        <f t="shared" si="2"/>
         <v>72</v>
       </c>
-      <c r="B88" s="16">
+      <c r="B88" s="14">
         <v>1.17</v>
       </c>
-      <c r="C88" s="17">
+      <c r="C88" s="15">
         <f>ROUND((C81*(B88^A88)), 0)</f>
         <v>1.93089129350047E+33</v>
       </c>
-      <c r="D88" s="17">
+      <c r="D88" s="15">
         <f>ROUND((D81*(B88^A88)), 0)</f>
         <v>3.11441647976616E+32</v>
       </c>
-      <c r="E88" s="17">
+      <c r="E88" s="15">
         <f>ROUND((E81*(B88^A88)), 0)</f>
         <v>1.17656048866748E+30</v>
       </c>
-      <c r="F88" s="17">
+      <c r="F88" s="15">
         <f>ROUND((F81*(B88^A88)), 0)</f>
         <v>1.3190549816281001E+22</v>
       </c>
-      <c r="G88" s="17"/>
-    </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A89" s="17">
-        <f t="shared" si="1"/>
+      <c r="G88" s="16">
+        <f>G81/(H88^A87)</f>
+        <v>4.6577597512054716E-2</v>
+      </c>
+      <c r="H88">
+        <v>1.006</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A89" s="15">
+        <f t="shared" si="2"/>
         <v>73</v>
       </c>
-      <c r="B89" s="16">
+      <c r="B89" s="14">
         <v>1.17</v>
       </c>
-      <c r="C89" s="17">
+      <c r="C89" s="15">
         <f>ROUND((C81*(B89^A89)), 0)</f>
         <v>2.2591428133955501E+33</v>
       </c>
-      <c r="D89" s="17">
+      <c r="D89" s="15">
         <f>ROUND((D81*(B89^A89)), 0)</f>
         <v>3.6438672813264004E+32</v>
       </c>
-      <c r="E89" s="17">
+      <c r="E89" s="15">
         <f>ROUND((E81*(B89^A89)), 0)</f>
         <v>1.37657577174095E+30</v>
       </c>
-      <c r="F89" s="17">
+      <c r="F89" s="15">
         <f>ROUND((F81*(B89^A89)), 0)</f>
         <v>1.5432943285048701E+22</v>
       </c>
-      <c r="G89" s="17"/>
-    </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A90" s="17">
-        <f t="shared" si="1"/>
+      <c r="G89" s="16">
+        <f>G81/(H89^A88)</f>
+        <v>4.6299798719736295E-2</v>
+      </c>
+      <c r="H89">
+        <v>1.006</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A90" s="15">
+        <f t="shared" si="2"/>
         <v>74</v>
       </c>
-      <c r="B90" s="16">
+      <c r="B90" s="14">
         <v>1.17</v>
       </c>
-      <c r="C90" s="17">
+      <c r="C90" s="15">
         <f>ROUND((C81*(B90^A90)), 0)</f>
         <v>2.6431970916728001E+33</v>
       </c>
-      <c r="D90" s="17">
+      <c r="D90" s="15">
         <f>ROUND((D81*(B90^A90)), 0)</f>
         <v>4.2633247191518899E+32</v>
       </c>
-      <c r="E90" s="17">
+      <c r="E90" s="15">
         <f>ROUND((E81*(B90^A90)), 0)</f>
         <v>1.6105936529369101E+30</v>
       </c>
-      <c r="F90" s="17">
+      <c r="F90" s="15">
         <f>ROUND((F81*(B90^A90)), 0)</f>
         <v>1.8056543643506999E+22</v>
       </c>
-      <c r="G90" s="17"/>
-    </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A91" s="17">
-        <f t="shared" si="1"/>
+      <c r="G90" s="16">
+        <f>G81/(H90^A89)</f>
+        <v>4.6023656779061922E-2</v>
+      </c>
+      <c r="H90">
+        <v>1.006</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A91" s="15">
+        <f t="shared" si="2"/>
         <v>75</v>
       </c>
-      <c r="B91" s="16">
+      <c r="B91" s="14">
         <v>1.17</v>
       </c>
-      <c r="C91" s="17">
+      <c r="C91" s="15">
         <f>ROUND((C81*(B91^A91)), 0)</f>
         <v>3.09254059725717E+33</v>
       </c>
-      <c r="D91" s="17">
+      <c r="D91" s="15">
         <f>ROUND((D81*(B91^A91)), 0)</f>
         <v>4.98808992140771E+32</v>
       </c>
-      <c r="E91" s="17">
+      <c r="E91" s="15">
         <f>ROUND((E81*(B91^A91)), 0)</f>
         <v>1.88439457393619E+30</v>
       </c>
-      <c r="F91" s="17">
+      <c r="F91" s="15">
         <f>ROUND((F81*(B91^A91)), 0)</f>
         <v>2.1126156062903201E+22</v>
       </c>
-      <c r="G91" s="17"/>
-    </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A92" s="17">
-        <f t="shared" si="1"/>
+      <c r="G91" s="16">
+        <f>G81/(H91^A90)</f>
+        <v>4.5749161808212653E-2</v>
+      </c>
+      <c r="H91">
+        <v>1.006</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A92" s="15">
+        <f t="shared" si="2"/>
         <v>76</v>
       </c>
-      <c r="B92" s="16">
+      <c r="B92" s="14">
         <v>1.17</v>
       </c>
-      <c r="C92" s="17">
+      <c r="C92" s="15">
         <f>ROUND((C81*(B92^A92)), 0)</f>
         <v>3.6182724987908899E+33</v>
       </c>
-      <c r="D92" s="17">
+      <c r="D92" s="15">
         <f>ROUND((D81*(B92^A92)), 0)</f>
         <v>5.8360652080470203E+32</v>
       </c>
-      <c r="E92" s="17">
+      <c r="E92" s="15">
         <f>ROUND((E81*(B92^A92)), 0)</f>
         <v>2.2047416515053399E+30</v>
       </c>
-      <c r="F92" s="17">
+      <c r="F92" s="15">
         <f>ROUND((F81*(B92^A92)), 0)</f>
         <v>2.4717602593596699E+22</v>
       </c>
-      <c r="G92" s="17"/>
-    </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A93" s="17">
-        <f t="shared" si="1"/>
+      <c r="G92" s="16">
+        <f>G81/(H92^A91)</f>
+        <v>4.5476303984306812E-2</v>
+      </c>
+      <c r="H92">
+        <v>1.006</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A93" s="15">
+        <f t="shared" si="2"/>
         <v>77</v>
       </c>
-      <c r="B93" s="16">
+      <c r="B93" s="14">
         <v>1.17</v>
       </c>
-      <c r="C93" s="17">
+      <c r="C93" s="15">
         <f>ROUND((C81*(B93^A93)), 0)</f>
         <v>4.2333788235853398E+33</v>
       </c>
-      <c r="D93" s="17">
+      <c r="D93" s="15">
         <f>ROUND((D81*(B93^A93)), 0)</f>
         <v>6.8281962934150107E+32</v>
       </c>
-      <c r="E93" s="17">
+      <c r="E93" s="15">
         <f>ROUND((E81*(B93^A93)), 0)</f>
         <v>2.5795477322612503E+30</v>
       </c>
-      <c r="F93" s="17">
+      <c r="F93" s="15">
         <f>ROUND((F81*(B93^A93)), 0)</f>
         <v>2.8919595034508198E+22</v>
       </c>
-      <c r="G93" s="17"/>
-    </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A94" s="17">
-        <f t="shared" si="1"/>
+      <c r="G93" s="16">
+        <f>G81/(H93^A92)</f>
+        <v>4.5205073543048514E-2</v>
+      </c>
+      <c r="H93">
+        <v>1.006</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A94" s="15">
+        <f t="shared" si="2"/>
         <v>78</v>
       </c>
-      <c r="B94" s="16">
+      <c r="B94" s="14">
         <v>1.17</v>
       </c>
-      <c r="C94" s="17">
+      <c r="C94" s="15">
         <f>ROUND((C81*(B94^A94)), 0)</f>
         <v>4.9530532235948502E+33</v>
       </c>
-      <c r="D94" s="17">
+      <c r="D94" s="15">
         <f>ROUND((D81*(B94^A94)), 0)</f>
         <v>7.9889896632955698E+32</v>
       </c>
-      <c r="E94" s="17">
+      <c r="E94" s="15">
         <f>ROUND((E81*(B94^A94)), 0)</f>
         <v>3.0180708467456598E+30</v>
       </c>
-      <c r="F94" s="17">
+      <c r="F94" s="15">
         <f>ROUND((F81*(B94^A94)), 0)</f>
         <v>3.3835926190374601E+22</v>
       </c>
-      <c r="G94" s="17"/>
-    </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A95" s="17">
-        <f t="shared" si="1"/>
+      <c r="G94" s="16">
+        <f>G81/(H94^A93)</f>
+        <v>4.4935460778378247E-2</v>
+      </c>
+      <c r="H94">
+        <v>1.006</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A95" s="15">
+        <f t="shared" si="2"/>
         <v>79</v>
       </c>
-      <c r="B95" s="16">
+      <c r="B95" s="14">
         <v>1.17</v>
       </c>
-      <c r="C95" s="17">
+      <c r="C95" s="15">
         <f>ROUND((C81*(B95^A95)), 0)</f>
         <v>5.7950722716059701E+33</v>
       </c>
-      <c r="D95" s="17">
+      <c r="D95" s="15">
         <f>ROUND((D81*(B95^A95)), 0)</f>
         <v>9.3471179060558104E+32</v>
       </c>
-      <c r="E95" s="17">
+      <c r="E95" s="15">
         <f>ROUND((E81*(B95^A95)), 0)</f>
         <v>3.5311428906924198E+30</v>
       </c>
-      <c r="F95" s="17">
+      <c r="F95" s="15">
         <f>ROUND((F81*(B95^A95)), 0)</f>
         <v>3.9588033642738196E+22</v>
       </c>
-      <c r="G95" s="17"/>
-    </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A96" s="17">
-        <f t="shared" si="1"/>
+      <c r="G95" s="16">
+        <f>G81/(H95^A94)</f>
+        <v>4.4667456042125492E-2</v>
+      </c>
+      <c r="H95">
+        <v>1.006</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A96" s="15">
+        <f t="shared" si="2"/>
         <v>80</v>
       </c>
-      <c r="B96" s="16">
+      <c r="B96" s="14">
         <v>1.17</v>
       </c>
-      <c r="C96" s="17">
+      <c r="C96" s="15">
         <f>ROUND((C81*(B96^A96)), 0)</f>
         <v>6.7802345577789906E+33</v>
       </c>
-      <c r="D96" s="17">
+      <c r="D96" s="15">
         <f>ROUND((D81*(B96^A96)), 0)</f>
         <v>1.09361279500853E+33</v>
       </c>
-      <c r="E96" s="17">
+      <c r="E96" s="15">
         <f>ROUND((E81*(B96^A96)), 0)</f>
         <v>4.1314371821101303E+30</v>
       </c>
-      <c r="F96" s="17">
+      <c r="F96" s="15">
         <f>ROUND((F81*(B96^A96)), 0)</f>
         <v>4.6317999362003698E+22</v>
       </c>
-      <c r="G96" s="17"/>
-    </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A97" s="17">
-        <f t="shared" si="1"/>
+      <c r="G96" s="16">
+        <f>G81/(H96^A95)</f>
+        <v>4.4401049743663518E-2</v>
+      </c>
+      <c r="H96">
+        <v>1.006</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A97" s="15">
+        <f t="shared" si="2"/>
         <v>81</v>
       </c>
-      <c r="B97" s="16">
+      <c r="B97" s="14">
         <v>1.1200000000000001</v>
       </c>
-      <c r="C97" s="17">
+      <c r="C97" s="15">
         <f>ROUND((C96*(B97^A97)), 0)</f>
         <v>6.5751331893077597E+37</v>
       </c>
-      <c r="D97" s="17">
+      <c r="D97" s="15">
         <f>ROUND((D96*(B97^A97)), 0)</f>
         <v>1.06053112520456E+37</v>
       </c>
-      <c r="E97" s="17">
+      <c r="E97" s="15">
         <f>ROUND((E96*(B97^A97)), 0)</f>
         <v>4.0064616502781901E+34</v>
       </c>
-      <c r="F97" s="17">
+      <c r="F97" s="15">
         <f>ROUND((F96*(B97^A97)), 0)</f>
         <v>4.4916884847005498E+26</v>
       </c>
-      <c r="G97" s="17"/>
-    </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A98" s="17">
-        <f t="shared" si="1"/>
+      <c r="G97" s="16">
+        <f>G96/(H97^A96)</f>
+        <v>3.7842124958675005E-2</v>
+      </c>
+      <c r="H97">
+        <v>1.002</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A98" s="15">
+        <f t="shared" si="2"/>
         <v>82</v>
       </c>
-      <c r="B98" s="16">
+      <c r="B98" s="14">
         <v>1.1200000000000001</v>
       </c>
-      <c r="C98" s="17">
+      <c r="C98" s="15">
         <f>ROUND((C96*(B98^A98)), 0)</f>
         <v>7.36414917202469E+37</v>
       </c>
-      <c r="D98" s="17">
+      <c r="D98" s="15">
         <f>ROUND((D96*(B98^A98)), 0)</f>
         <v>1.18779486022911E+37</v>
       </c>
-      <c r="E98" s="17">
+      <c r="E98" s="15">
         <f>ROUND((E96*(B98^A98)), 0)</f>
         <v>4.4872370483115796E+34</v>
       </c>
-      <c r="F98" s="17">
+      <c r="F98" s="15">
         <f>ROUND((F96*(B98^A98)), 0)</f>
         <v>5.0306911028646203E+26</v>
       </c>
-      <c r="G98" s="17"/>
-    </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A99" s="17">
-        <f t="shared" si="1"/>
+      <c r="G98" s="16">
+        <f>G96/(H98^A97)</f>
+        <v>3.7766591775124751E-2</v>
+      </c>
+      <c r="H98">
+        <v>1.002</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A99" s="15">
+        <f t="shared" si="2"/>
         <v>83</v>
       </c>
-      <c r="B99" s="16">
+      <c r="B99" s="14">
         <v>1.1200000000000001</v>
       </c>
-      <c r="C99" s="17">
+      <c r="C99" s="15">
         <f>ROUND((C96*(B99^A99)), 0)</f>
         <v>8.2478470726676497E+37</v>
       </c>
-      <c r="D99" s="17">
+      <c r="D99" s="15">
         <f>ROUND((D96*(B99^A99)), 0)</f>
         <v>1.3303302434566E+37</v>
       </c>
-      <c r="E99" s="17">
+      <c r="E99" s="15">
         <f>ROUND((E96*(B99^A99)), 0)</f>
         <v>5.0257054941089702E+34</v>
       </c>
-      <c r="F99" s="17">
+      <c r="F99" s="15">
         <f>ROUND((F96*(B99^A99)), 0)</f>
         <v>5.6343740352083701E+26</v>
       </c>
-      <c r="G99" s="17"/>
-    </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A100" s="17">
-        <f t="shared" si="1"/>
+      <c r="G99" s="16">
+        <f>G96/(H99^A98)</f>
+        <v>3.7691209356411938E-2</v>
+      </c>
+      <c r="H99">
+        <v>1.002</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A100" s="15">
+        <f t="shared" si="2"/>
         <v>84</v>
       </c>
-      <c r="B100" s="16">
+      <c r="B100" s="14">
         <v>1.1200000000000001</v>
       </c>
-      <c r="C100" s="17">
+      <c r="C100" s="15">
         <f>ROUND((C96*(B100^A100)), 0)</f>
         <v>9.2375887213877696E+37</v>
       </c>
-      <c r="D100" s="17">
+      <c r="D100" s="15">
         <f>ROUND((D96*(B100^A100)), 0)</f>
         <v>1.4899698726714001E+37</v>
       </c>
-      <c r="E100" s="17">
+      <c r="E100" s="15">
         <f>ROUND((E96*(B100^A100)), 0)</f>
         <v>5.6287901534020404E+34</v>
       </c>
-      <c r="F100" s="17">
+      <c r="F100" s="15">
         <f>ROUND((F96*(B100^A100)), 0)</f>
         <v>6.31049891943337E+26</v>
       </c>
-      <c r="G100" s="17"/>
-    </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A101" s="17">
-        <f t="shared" si="1"/>
+      <c r="G100" s="16">
+        <f>G96/(H100^A99)</f>
+        <v>3.7615977401608713E-2</v>
+      </c>
+      <c r="H100">
+        <v>1.002</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A101" s="15">
+        <f t="shared" si="2"/>
         <v>85</v>
       </c>
-      <c r="B101" s="16">
+      <c r="B101" s="14">
         <v>1.1200000000000001</v>
       </c>
-      <c r="C101" s="17">
+      <c r="C101" s="15">
         <f>ROUND((C96*(B101^A101)), 0)</f>
         <v>1.0346099367954299E+38</v>
       </c>
-      <c r="D101" s="17">
+      <c r="D101" s="15">
         <f>ROUND((D96*(B101^A101)), 0)</f>
         <v>1.66876625739196E+37</v>
       </c>
-      <c r="E101" s="17">
+      <c r="E101" s="15">
         <f>ROUND((E96*(B101^A101)), 0)</f>
         <v>6.3042449718102899E+34</v>
       </c>
-      <c r="F101" s="17">
+      <c r="F101" s="15">
         <f>ROUND((F96*(B101^A101)), 0)</f>
         <v>7.0677587897653797E+26</v>
       </c>
-      <c r="G101" s="17"/>
-    </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A102" s="17">
-        <f t="shared" si="1"/>
+      <c r="G101" s="16">
+        <f>G96/(H101^A100)</f>
+        <v>3.7540895610387932E-2</v>
+      </c>
+      <c r="H101">
+        <v>1.002</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A102" s="15">
+        <f t="shared" si="2"/>
         <v>86</v>
       </c>
-      <c r="B102" s="16">
+      <c r="B102" s="14">
         <v>1.1200000000000001</v>
       </c>
-      <c r="C102" s="17">
+      <c r="C102" s="15">
         <f>ROUND((C96*(B102^A102)), 0)</f>
         <v>1.15876312921088E+38</v>
       </c>
-      <c r="D102" s="17">
+      <c r="D102" s="15">
         <f>ROUND((D96*(B102^A102)), 0)</f>
         <v>1.8690182082790001E+37</v>
       </c>
-      <c r="E102" s="17">
+      <c r="E102" s="15">
         <f>ROUND((E96*(B102^A102)), 0)</f>
         <v>7.06075436842752E+34</v>
       </c>
-      <c r="F102" s="17">
+      <c r="F102" s="15">
         <f>ROUND((F96*(B102^A102)), 0)</f>
         <v>7.9158898445372294E+26</v>
       </c>
-      <c r="G102" s="17"/>
-    </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A103" s="17">
-        <f t="shared" si="1"/>
+      <c r="G102" s="16">
+        <f>G96/(H102^A101)</f>
+        <v>3.7465963683021894E-2</v>
+      </c>
+      <c r="H102">
+        <v>1.002</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A103" s="15">
+        <f t="shared" si="2"/>
         <v>87</v>
       </c>
-      <c r="B103" s="16">
+      <c r="B103" s="14">
         <v>1.1200000000000001</v>
       </c>
-      <c r="C103" s="17">
+      <c r="C103" s="15">
         <f>ROUND((C96*(B103^A103)), 0)</f>
         <v>1.2978147047161901E+38</v>
       </c>
-      <c r="D103" s="17">
+      <c r="D103" s="15">
         <f>ROUND((D96*(B103^A103)), 0)</f>
         <v>2.0933003932724801E+37</v>
       </c>
-      <c r="E103" s="17">
+      <c r="E103" s="15">
         <f>ROUND((E96*(B103^A103)), 0)</f>
         <v>7.9080448926388197E+34</v>
       </c>
-      <c r="F103" s="17">
+      <c r="F103" s="15">
         <f>ROUND((F96*(B103^A103)), 0)</f>
         <v>8.8657966258816902E+26</v>
       </c>
-      <c r="G103" s="17"/>
-    </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A104" s="17">
-        <f t="shared" si="1"/>
+      <c r="G103" s="16">
+        <f>G96/(H103^A102)</f>
+        <v>3.7391181320381141E-2</v>
+      </c>
+      <c r="H103">
+        <v>1.002</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A104" s="15">
+        <f t="shared" si="2"/>
         <v>88</v>
       </c>
-      <c r="B104" s="16">
+      <c r="B104" s="14">
         <v>1.1200000000000001</v>
       </c>
-      <c r="C104" s="17">
+      <c r="C104" s="15">
         <f>ROUND((C96*(B104^A104)), 0)</f>
         <v>1.4535524692821301E+38</v>
       </c>
-      <c r="D104" s="17">
+      <c r="D104" s="15">
         <f>ROUND((D96*(B104^A104)), 0)</f>
         <v>2.3444964404651799E+37</v>
       </c>
-      <c r="E104" s="17">
+      <c r="E104" s="15">
         <f>ROUND((E96*(B104^A104)), 0)</f>
         <v>8.8570102797554793E+34</v>
       </c>
-      <c r="F104" s="17">
+      <c r="F104" s="15">
         <f>ROUND((F96*(B104^A104)), 0)</f>
         <v>9.9296922209874995E+26</v>
       </c>
-      <c r="G104" s="17"/>
-    </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A105" s="17">
-        <f t="shared" si="1"/>
+      <c r="G104" s="16">
+        <f>G96/(H104^A103)</f>
+        <v>3.7316548223933273E-2</v>
+      </c>
+      <c r="H104">
+        <v>1.002</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A105" s="15">
+        <f t="shared" si="2"/>
         <v>89</v>
       </c>
-      <c r="B105" s="16">
+      <c r="B105" s="14">
         <v>1.1200000000000001</v>
       </c>
-      <c r="C105" s="17">
+      <c r="C105" s="15">
         <f>ROUND((C96*(B105^A105)), 0)</f>
         <v>1.6279787655959899E+38</v>
       </c>
-      <c r="D105" s="17">
+      <c r="D105" s="15">
         <f>ROUND((D96*(B105^A105)), 0)</f>
         <v>2.6258360133209999E+37</v>
       </c>
-      <c r="E105" s="17">
+      <c r="E105" s="15">
         <f>ROUND((E96*(B105^A105)), 0)</f>
         <v>9.9198515133261402E+34</v>
       </c>
-      <c r="F105" s="17">
+      <c r="F105" s="15">
         <f>ROUND((F96*(B105^A105)), 0)</f>
         <v>1.1121255287506001E+27</v>
       </c>
-      <c r="G105" s="17"/>
-    </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A106" s="17">
-        <f t="shared" si="1"/>
+      <c r="G105" s="16">
+        <f>G96/(H105^A104)</f>
+        <v>3.7242064095741788E-2</v>
+      </c>
+      <c r="H105">
+        <v>1.002</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A106" s="15">
+        <f t="shared" si="2"/>
         <v>90</v>
       </c>
-      <c r="B106" s="16">
+      <c r="B106" s="14">
         <v>1.1200000000000001</v>
       </c>
-      <c r="C106" s="17">
+      <c r="C106" s="15">
         <f>ROUND((C96*(B106^A106)), 0)</f>
         <v>1.8233362174675099E+38</v>
       </c>
-      <c r="D106" s="17">
+      <c r="D106" s="15">
         <f>ROUND((D96*(B106^A106)), 0)</f>
         <v>2.9409363349195201E+37</v>
       </c>
-      <c r="E106" s="17">
+      <c r="E106" s="15">
         <f>ROUND((E96*(B106^A106)), 0)</f>
         <v>1.1110233694925301E+35</v>
       </c>
-      <c r="F106" s="17">
+      <c r="F106" s="15">
         <f>ROUND((F96*(B106^A106)), 0)</f>
         <v>1.24558059220067E+27</v>
       </c>
-      <c r="G106" s="17"/>
-    </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A107" s="17">
-        <f t="shared" si="1"/>
+      <c r="G106" s="16">
+        <f>G96/(H106^A105)</f>
+        <v>3.7167728638464848E-2</v>
+      </c>
+      <c r="H106">
+        <v>1.002</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A107" s="15">
+        <f t="shared" si="2"/>
         <v>91</v>
       </c>
-      <c r="B107" s="16">
+      <c r="B107" s="14">
         <v>1.1200000000000001</v>
       </c>
-      <c r="C107" s="17">
+      <c r="C107" s="15">
         <f>ROUND((C96*(B107^A107)), 0)</f>
         <v>2.04213656356361E+38</v>
       </c>
-      <c r="D107" s="17">
+      <c r="D107" s="15">
         <f>ROUND((D96*(B107^A107)), 0)</f>
         <v>3.2938486951098599E+37</v>
       </c>
-      <c r="E107" s="17">
+      <c r="E107" s="15">
         <f>ROUND((E96*(B107^A107)), 0)</f>
         <v>1.24434617383163E+35</v>
       </c>
-      <c r="F107" s="17">
+      <c r="F107" s="15">
         <f>ROUND((F96*(B107^A107)), 0)</f>
         <v>1.3950502632647499E+27</v>
       </c>
-      <c r="G107" s="17"/>
-    </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A108" s="17">
-        <f t="shared" si="1"/>
+      <c r="G107" s="16">
+        <f>G96/(H107^A106)</f>
+        <v>3.7093541555354152E-2</v>
+      </c>
+      <c r="H107">
+        <v>1.002</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A108" s="15">
+        <f t="shared" si="2"/>
         <v>92</v>
       </c>
-      <c r="B108" s="16">
+      <c r="B108" s="14">
         <v>1.1200000000000001</v>
       </c>
-      <c r="C108" s="17">
+      <c r="C108" s="15">
         <f>ROUND((C96*(B108^A108)), 0)</f>
         <v>2.2871929511912402E+38</v>
       </c>
-      <c r="D108" s="17">
+      <c r="D108" s="15">
         <f>ROUND((D96*(B108^A108)), 0)</f>
         <v>3.6891105385230399E+37</v>
       </c>
-      <c r="E108" s="17">
+      <c r="E108" s="15">
         <f>ROUND((E96*(B108^A108)), 0)</f>
         <v>1.39366771469143E+35</v>
       </c>
-      <c r="F108" s="17">
+      <c r="F108" s="15">
         <f>ROUND((F96*(B108^A108)), 0)</f>
         <v>1.5624562948565199E+27</v>
       </c>
-      <c r="G108" s="17"/>
-    </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A109" s="17">
-        <f t="shared" si="1"/>
+      <c r="G108" s="16">
+        <f>G96/(H108^A107)</f>
+        <v>3.7019502550253644E-2</v>
+      </c>
+      <c r="H108">
+        <v>1.002</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A109" s="15">
+        <f t="shared" si="2"/>
         <v>93</v>
       </c>
-      <c r="B109" s="16">
+      <c r="B109" s="14">
         <v>1.1200000000000001</v>
       </c>
-      <c r="C109" s="17">
+      <c r="C109" s="15">
         <f>ROUND((C96*(B109^A109)), 0)</f>
         <v>2.56165610533419E+38</v>
       </c>
-      <c r="D109" s="17">
+      <c r="D109" s="15">
         <f>ROUND((D96*(B109^A109)), 0)</f>
         <v>4.13180380314581E+37</v>
       </c>
-      <c r="E109" s="17">
+      <c r="E109" s="15">
         <f>ROUND((E96*(B109^A109)), 0)</f>
         <v>1.5609078404544E+35</v>
       </c>
-      <c r="F109" s="17">
+      <c r="F109" s="15">
         <f>ROUND((F96*(B109^A109)), 0)</f>
         <v>1.7499510502393099E+27</v>
       </c>
-      <c r="G109" s="17"/>
-    </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A110" s="17">
-        <f t="shared" si="1"/>
+      <c r="G109" s="16">
+        <f>G96/(H109^A108)</f>
+        <v>3.6945611327598445E-2</v>
+      </c>
+      <c r="H109">
+        <v>1.002</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A110" s="15">
+        <f t="shared" si="2"/>
         <v>94</v>
       </c>
-      <c r="B110" s="16">
+      <c r="B110" s="14">
         <v>1.1200000000000001</v>
       </c>
-      <c r="C110" s="17">
+      <c r="C110" s="15">
         <f>ROUND((C96*(B110^A110)), 0)</f>
         <v>2.8690548379742898E+38</v>
       </c>
-      <c r="D110" s="17">
+      <c r="D110" s="15">
         <f>ROUND((D96*(B110^A110)), 0)</f>
         <v>4.6276202595233002E+37</v>
       </c>
-      <c r="E110" s="17">
+      <c r="E110" s="15">
         <f>ROUND((E96*(B110^A110)), 0)</f>
         <v>1.7482167813089301E+35</v>
       </c>
-      <c r="F110" s="17">
+      <c r="F110" s="15">
         <f>ROUND((F96*(B110^A110)), 0)</f>
         <v>1.9599451762680199E+27</v>
       </c>
-      <c r="G110" s="17"/>
-    </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A111" s="17">
-        <f t="shared" si="1"/>
+      <c r="G110" s="16">
+        <f>G96/(H110^A109)</f>
+        <v>3.6871867592413614E-2</v>
+      </c>
+      <c r="H110">
+        <v>1.002</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A111" s="15">
+        <f t="shared" si="2"/>
         <v>95</v>
       </c>
-      <c r="B111" s="16">
+      <c r="B111" s="14">
         <v>1.1200000000000001</v>
       </c>
-      <c r="C111" s="17">
+      <c r="C111" s="15">
         <f>ROUND((C96*(B111^A111)), 0)</f>
         <v>3.2133414185312101E+38</v>
       </c>
-      <c r="D111" s="17">
+      <c r="D111" s="15">
         <f>ROUND((D96*(B111^A111)), 0)</f>
         <v>5.1829346906661003E+37</v>
       </c>
-      <c r="E111" s="17">
+      <c r="E111" s="15">
         <f>ROUND((E96*(B111^A111)), 0)</f>
         <v>1.9580027950660001E+35</v>
       </c>
-      <c r="F111" s="17">
+      <c r="F111" s="15">
         <f>ROUND((F96*(B111^A111)), 0)</f>
         <v>2.1951385974201901E+27</v>
       </c>
-      <c r="G111" s="17"/>
-    </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A112" s="17">
-        <f t="shared" si="1"/>
+      <c r="G111" s="16">
+        <f>G96/(H111^A110)</f>
+        <v>3.6798271050313011E-2</v>
+      </c>
+      <c r="H111">
+        <v>1.002</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A112" s="15">
+        <f t="shared" si="2"/>
         <v>96</v>
       </c>
-      <c r="B112" s="16">
+      <c r="B112" s="14">
         <v>1.07</v>
       </c>
-      <c r="C112" s="17">
+      <c r="C112" s="15">
         <f>ROUND((C111*(B112^A112)), 0)</f>
         <v>2.12715692388953E+41</v>
       </c>
-      <c r="D112" s="17">
+      <c r="D112" s="15">
         <f>ROUND((D111*(B112^A112)), 0)</f>
         <v>3.4309816410224501E+40</v>
       </c>
-      <c r="E112" s="17">
+      <c r="E112" s="15">
         <f>ROUND((E111*(B112^A112)), 0)</f>
         <v>1.2961520921805601E+38</v>
       </c>
-      <c r="F112" s="17">
+      <c r="F112" s="15">
         <f>ROUND((F111*(B112^A112)), 0)</f>
         <v>1.4531304515204101E+30</v>
       </c>
-      <c r="G112" s="17"/>
-    </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A113" s="17">
-        <f t="shared" si="1"/>
+      <c r="G112" s="16">
+        <f>G111/(H112^A111)</f>
+        <v>3.3464940216410513E-2</v>
+      </c>
+      <c r="H112">
+        <v>1.0009999999999999</v>
+      </c>
+    </row>
+    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A113" s="15">
+        <f t="shared" si="2"/>
         <v>97</v>
       </c>
-      <c r="B113" s="16">
+      <c r="B113" s="14">
         <v>1.07</v>
       </c>
-      <c r="C113" s="17">
+      <c r="C113" s="15">
         <f>ROUND((C111*(B113^A113)), 0)</f>
         <v>2.2760579085617902E+41</v>
       </c>
-      <c r="D113" s="17">
+      <c r="D113" s="15">
         <f>ROUND((D111*(B113^A113)), 0)</f>
         <v>3.6711503558940202E+40</v>
       </c>
-      <c r="E113" s="17">
+      <c r="E113" s="15">
         <f>ROUND((E111*(B113^A113)), 0)</f>
         <v>1.3868827386332E+38</v>
       </c>
-      <c r="F113" s="17">
+      <c r="F113" s="15">
         <f>ROUND((F111*(B113^A113)), 0)</f>
         <v>1.55484958312684E+30</v>
       </c>
-      <c r="G113" s="17"/>
-    </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A114" s="17">
-        <f t="shared" si="1"/>
+      <c r="G113" s="16">
+        <f>G111/(H113^A112)</f>
+        <v>3.3431508707702819E-2</v>
+      </c>
+      <c r="H113">
+        <v>1.0009999999999999</v>
+      </c>
+    </row>
+    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A114" s="15">
+        <f t="shared" si="2"/>
         <v>98</v>
       </c>
-      <c r="B114" s="16">
+      <c r="B114" s="14">
         <v>1.07</v>
       </c>
-      <c r="C114" s="17">
+      <c r="C114" s="15">
         <f>ROUND((C111*(B114^A114)), 0)</f>
         <v>2.4353819621611201E+41</v>
       </c>
-      <c r="D114" s="17">
+      <c r="D114" s="15">
         <f>ROUND((D111*(B114^A114)), 0)</f>
         <v>3.9281308808066001E+40</v>
       </c>
-      <c r="E114" s="17">
+      <c r="E114" s="15">
         <f>ROUND((E111*(B114^A114)), 0)</f>
         <v>1.48396453033753E+38</v>
       </c>
-      <c r="F114" s="17">
+      <c r="F114" s="15">
         <f>ROUND((F111*(B114^A114)), 0)</f>
         <v>1.66368905394572E+30</v>
       </c>
-      <c r="G114" s="17"/>
-    </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A115" s="17">
-        <f t="shared" si="1"/>
+      <c r="G114" s="16">
+        <f>G111/(H114^A113)</f>
+        <v>3.3398110597105714E-2</v>
+      </c>
+      <c r="H114">
+        <v>1.0009999999999999</v>
+      </c>
+    </row>
+    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A115" s="15">
+        <f t="shared" si="2"/>
         <v>99</v>
       </c>
-      <c r="B115" s="16">
+      <c r="B115" s="14">
         <v>1.07</v>
       </c>
-      <c r="C115" s="17">
+      <c r="C115" s="15">
         <f>ROUND((C111*(B115^A115)), 0)</f>
         <v>2.6058586995123999E+41</v>
       </c>
-      <c r="D115" s="17">
+      <c r="D115" s="15">
         <f>ROUND((D111*(B115^A115)), 0)</f>
         <v>4.2031000424630699E+40</v>
       </c>
-      <c r="E115" s="17">
+      <c r="E115" s="15">
         <f>ROUND((E111*(B115^A115)), 0)</f>
         <v>1.5878420474611499E+38</v>
       </c>
-      <c r="F115" s="17">
+      <c r="F115" s="15">
         <f>ROUND((F111*(B115^A115)), 0)</f>
         <v>1.7801472877219199E+30</v>
       </c>
-      <c r="G115" s="17"/>
-    </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A116" s="17">
-        <f t="shared" si="1"/>
+      <c r="G115" s="16">
+        <f>G111/(H115^A114)</f>
+        <v>3.3364745851254471E-2</v>
+      </c>
+      <c r="H115">
+        <v>1.0009999999999999</v>
+      </c>
+    </row>
+    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A116" s="15">
+        <f t="shared" si="2"/>
         <v>100</v>
       </c>
-      <c r="B116" s="16">
+      <c r="B116" s="14">
         <v>1.07</v>
       </c>
-      <c r="C116" s="17">
+      <c r="C116" s="15">
         <f>ROUND((C111*(B116^A116)), 0)</f>
         <v>2.7882688084782698E+41</v>
       </c>
-      <c r="D116" s="17">
+      <c r="D116" s="15">
         <f>ROUND((D111*(B116^A116)), 0)</f>
         <v>4.4973170454354798E+40</v>
       </c>
-      <c r="E116" s="17">
+      <c r="E116" s="15">
         <f>ROUND((E111*(B116^A116)), 0)</f>
         <v>1.6989909907834399E+38</v>
       </c>
-      <c r="F116" s="17">
+      <c r="F116" s="15">
         <f>ROUND((F111*(B116^A116)), 0)</f>
         <v>1.9047575978624599E+30</v>
       </c>
-      <c r="G116" s="17"/>
-    </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G116" s="16">
+        <f>G111/(H116^A115)</f>
+        <v>3.3331414436817655E-2</v>
+      </c>
+      <c r="H116">
+        <v>1.0009999999999999</v>
+      </c>
+    </row>
+    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>101</v>
       </c>
-      <c r="B117" s="16">
+      <c r="B117" s="14">
         <v>1.03</v>
       </c>
-      <c r="C117" s="17">
+      <c r="C117" s="15">
         <f>ROUND((C116*(B117^A117)), 0)</f>
         <v>5.5194313456659598E+42</v>
       </c>
-      <c r="D117" s="17">
+      <c r="D117" s="15">
         <f>ROUND((D116*(B117^A117)), 0)</f>
         <v>8.90252496333798E+41</v>
       </c>
-      <c r="E117" s="17">
+      <c r="E117" s="15">
         <f>ROUND((E116*(B117^A117)), 0)</f>
         <v>3.3631851068376897E+39</v>
       </c>
-      <c r="F117" s="17">
+      <c r="F117" s="15">
         <f>ROUND((F116*(B117^A117)), 0)</f>
         <v>3.7705040344640099E+31</v>
+      </c>
+      <c r="G117" s="16">
+        <f>G116/(H117^A116)</f>
+        <v>3.076975760649792E-2</v>
+      </c>
+      <c r="H117">
+        <v>1.0007999999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added some Tooltips for Number Display and fixed display of Numbers
</commit_message>
<xml_diff>
--- a/public/Level.xlsx
+++ b/public/Level.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kevin Zeugs\Studium\Free_Projects\idle_alphabet\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36CBCDD3-7292-4404-8B43-5BF08EFCE8F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00AFCDBD-D7A0-4205-A8BA-A325D69640A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{EE7CB22D-DBB3-4CC5-A134-0A5565C2D036}"/>
   </bookViews>
@@ -679,8 +679,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F719A59D-A330-4459-AA9A-D2893BAE4388}">
   <dimension ref="A1:FE117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D53" sqref="D53"/>
+    <sheetView tabSelected="1" topLeftCell="D70" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="J51" sqref="J51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3756,7 +3756,7 @@
         <v>1.07</v>
       </c>
       <c r="I25" s="14">
-        <f t="shared" si="1"/>
+        <f>J25*(B25^A24)</f>
         <v>4.2998169599999994</v>
       </c>
       <c r="J25">
@@ -4686,7 +4686,7 @@
         <v>1.0149999999999999</v>
       </c>
       <c r="I52" s="14">
-        <f t="shared" si="1"/>
+        <f>J52*(B52^A51)</f>
         <v>42956730098969.508</v>
       </c>
       <c r="J52" s="14">

</xml_diff>

<commit_message>
Working on optimising and fixing Rate & Costs Calculations. Did some Prework for implementation of Prestige System !
</commit_message>
<xml_diff>
--- a/public/Level.xlsx
+++ b/public/Level.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kevin Zeugs\Studium\Free_Projects\idle_alphabet\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00AFCDBD-D7A0-4205-A8BA-A325D69640A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{576049A3-BF8D-439F-B511-0565A553D43D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{EE7CB22D-DBB3-4CC5-A134-0A5565C2D036}"/>
+    <workbookView xWindow="-19200" yWindow="-15" windowWidth="19200" windowHeight="21000" activeTab="1" xr2:uid="{EE7CB22D-DBB3-4CC5-A134-0A5565C2D036}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="773" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="782" uniqueCount="63">
   <si>
     <t>Basisliste</t>
   </si>
@@ -208,13 +209,33 @@
   <si>
     <t>Rate Init</t>
   </si>
+  <si>
+    <t>Costs</t>
+  </si>
+  <si>
+    <t>Growth Rate Costs</t>
+  </si>
+  <si>
+    <t>Growth Rate Prod</t>
+  </si>
+  <si>
+    <t>Production</t>
+  </si>
+  <si>
+    <t>Differenz Costs to Production</t>
+  </si>
+  <si>
+    <t>Prestige Points</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="#,##0.0000000000000000"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="166" formatCode="#,##0.00_ ;[Red]\-#,##0.00\ "/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -331,7 +352,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -363,6 +384,10 @@
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -679,7 +704,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F719A59D-A330-4459-AA9A-D2893BAE4388}">
   <dimension ref="A1:FE117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D70" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="J51" sqref="J51"/>
     </sheetView>
   </sheetViews>
@@ -6875,4 +6900,2755 @@
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49322D13-1AA9-459B-8DB6-87D7646DC160}">
+  <dimension ref="A1:L76"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.42578125" style="18"/>
+    <col min="2" max="2" width="17.28515625" style="19" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="20.42578125" style="14" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" style="19" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" style="17" customWidth="1"/>
+    <col min="7" max="7" width="20.42578125" style="17" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="27.28515625" style="20" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.85546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="E1" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="F1" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="H1" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="K1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="18">
+        <v>1</v>
+      </c>
+      <c r="B2" s="19">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C2" s="14">
+        <v>2</v>
+      </c>
+      <c r="E2" s="19">
+        <v>1.2</v>
+      </c>
+      <c r="F2" s="17">
+        <v>1</v>
+      </c>
+      <c r="H2" s="20">
+        <f t="shared" ref="H2:H33" si="0">F2-C2</f>
+        <v>-1</v>
+      </c>
+      <c r="I2" s="20">
+        <f>F2-C2</f>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="18">
+        <f>A2+1</f>
+        <v>2</v>
+      </c>
+      <c r="B3" s="19">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C3" s="14">
+        <f>C2*POWER(B3,A2)</f>
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="D3" s="14">
+        <f>C2*POWER(B3,A2 - L3)</f>
+        <v>1.6528925619834709</v>
+      </c>
+      <c r="E3" s="19">
+        <v>1.2</v>
+      </c>
+      <c r="F3" s="14">
+        <f>F2*POWER(E3,A3)</f>
+        <v>1.44</v>
+      </c>
+      <c r="G3" s="14">
+        <f>F2*POWER(E3,(A3 + L4))</f>
+        <v>1.728</v>
+      </c>
+      <c r="H3" s="20">
+        <f t="shared" si="0"/>
+        <v>-0.76000000000000023</v>
+      </c>
+      <c r="I3" s="20">
+        <f>G3-D3</f>
+        <v>7.5107438016529082E-2</v>
+      </c>
+      <c r="K3" t="s">
+        <v>57</v>
+      </c>
+      <c r="L3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="18">
+        <f t="shared" ref="A4:A67" si="1">A3+1</f>
+        <v>3</v>
+      </c>
+      <c r="B4" s="19">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C4" s="14">
+        <f>C2*POWER(B4,A3)</f>
+        <v>2.4200000000000004</v>
+      </c>
+      <c r="D4" s="14">
+        <f>C2*POWER(B4,A3 - L3)</f>
+        <v>1.8181818181818181</v>
+      </c>
+      <c r="E4" s="19">
+        <v>1.2</v>
+      </c>
+      <c r="F4" s="14">
+        <f>F2*POWER(E4,A4)</f>
+        <v>1.728</v>
+      </c>
+      <c r="G4" s="14">
+        <f>F2*POWER(E4,(A4 + L4))</f>
+        <v>2.0735999999999999</v>
+      </c>
+      <c r="H4" s="20">
+        <f t="shared" si="0"/>
+        <v>-0.69200000000000039</v>
+      </c>
+      <c r="I4" s="20">
+        <f t="shared" ref="I4:I67" si="2">G4-D4</f>
+        <v>0.25541818181818177</v>
+      </c>
+      <c r="K4" t="s">
+        <v>60</v>
+      </c>
+      <c r="L4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="18">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="B5" s="19">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C5" s="14">
+        <f>C2*POWER(B5,A4)</f>
+        <v>2.6620000000000008</v>
+      </c>
+      <c r="D5" s="14">
+        <f>C2*POWER(B5,A4 - L3)</f>
+        <v>2</v>
+      </c>
+      <c r="E5" s="19">
+        <v>1.2</v>
+      </c>
+      <c r="F5" s="14">
+        <f>F2*POWER(E5,A5)</f>
+        <v>2.0735999999999999</v>
+      </c>
+      <c r="G5" s="14">
+        <f>F2*POWER(E5,(A5 + L4))</f>
+        <v>2.4883199999999999</v>
+      </c>
+      <c r="H5" s="20">
+        <f t="shared" si="0"/>
+        <v>-0.58840000000000092</v>
+      </c>
+      <c r="I5" s="20">
+        <f t="shared" si="2"/>
+        <v>0.48831999999999987</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="18">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="B6" s="19">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C6" s="14">
+        <f>C2*POWER(B6,A5)</f>
+        <v>2.9282000000000008</v>
+      </c>
+      <c r="D6" s="14">
+        <f>C2*POWER(B6,A5 - L3)</f>
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="E6" s="19">
+        <v>1.2</v>
+      </c>
+      <c r="F6" s="14">
+        <f>F2*POWER(E6,A6)</f>
+        <v>2.4883199999999999</v>
+      </c>
+      <c r="G6" s="14">
+        <f>F2*POWER(E6,(A6 + L4))</f>
+        <v>2.9859839999999997</v>
+      </c>
+      <c r="H6" s="20">
+        <f t="shared" si="0"/>
+        <v>-0.43988000000000094</v>
+      </c>
+      <c r="I6" s="20">
+        <f t="shared" si="2"/>
+        <v>0.78598399999999957</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="18">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="B7" s="19">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C7" s="14">
+        <f>C2*POWER(B7,A6)</f>
+        <v>3.2210200000000011</v>
+      </c>
+      <c r="D7" s="14">
+        <f>C2*POWER(B7,A6 - L3)</f>
+        <v>2.4200000000000004</v>
+      </c>
+      <c r="E7" s="19">
+        <v>1.2</v>
+      </c>
+      <c r="F7" s="14">
+        <f>F2*POWER(E7,A7)</f>
+        <v>2.9859839999999997</v>
+      </c>
+      <c r="G7" s="14">
+        <f>F2*POWER(E7,(A7 + L4))</f>
+        <v>3.5831807999999996</v>
+      </c>
+      <c r="H7" s="20">
+        <f t="shared" si="0"/>
+        <v>-0.23503600000000135</v>
+      </c>
+      <c r="I7" s="20">
+        <f t="shared" si="2"/>
+        <v>1.1631807999999992</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="18">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="B8" s="19">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C8" s="14">
+        <f>C2*POWER(B8,A7)</f>
+        <v>3.5431220000000017</v>
+      </c>
+      <c r="D8" s="14">
+        <f>C2*POWER(B8,A7 - L3)</f>
+        <v>2.6620000000000008</v>
+      </c>
+      <c r="E8" s="19">
+        <v>1.2</v>
+      </c>
+      <c r="F8" s="14">
+        <f>F2*POWER(E8,A8)</f>
+        <v>3.5831807999999996</v>
+      </c>
+      <c r="G8" s="14">
+        <f>F2*POWER(E8,(A8 + L4))</f>
+        <v>4.2998169599999994</v>
+      </c>
+      <c r="H8" s="20">
+        <f t="shared" si="0"/>
+        <v>4.0058799999997952E-2</v>
+      </c>
+      <c r="I8" s="20">
+        <f t="shared" si="2"/>
+        <v>1.6378169599999985</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="18">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="B9" s="19">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C9" s="14">
+        <f>C2*POWER(B9,A8)</f>
+        <v>3.8974342000000024</v>
+      </c>
+      <c r="D9" s="14">
+        <f>C2*POWER(B9,A8 - L3)</f>
+        <v>2.9282000000000008</v>
+      </c>
+      <c r="E9" s="19">
+        <v>1.2</v>
+      </c>
+      <c r="F9" s="14">
+        <f>F2*POWER(E9,A9)</f>
+        <v>4.2998169599999994</v>
+      </c>
+      <c r="G9" s="14">
+        <f>F2*POWER(E9,(A9 + L4))</f>
+        <v>5.1597803519999994</v>
+      </c>
+      <c r="H9" s="20">
+        <f t="shared" si="0"/>
+        <v>0.40238275999999695</v>
+      </c>
+      <c r="I9" s="20">
+        <f t="shared" si="2"/>
+        <v>2.2315803519999986</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="18">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="B10" s="19">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C10" s="14">
+        <f>C2*POWER(B10,A9)</f>
+        <v>4.2871776200000022</v>
+      </c>
+      <c r="D10" s="14">
+        <f>C2*POWER(B10,A9 - L3)</f>
+        <v>3.2210200000000011</v>
+      </c>
+      <c r="E10" s="19">
+        <v>1.2</v>
+      </c>
+      <c r="F10" s="14">
+        <f>F2*POWER(E10,A10)</f>
+        <v>5.1597803519999994</v>
+      </c>
+      <c r="G10" s="14">
+        <f>F2*POWER(E10,(A10 + L4))</f>
+        <v>6.1917364223999991</v>
+      </c>
+      <c r="H10" s="20">
+        <f t="shared" si="0"/>
+        <v>0.87260273199999716</v>
+      </c>
+      <c r="I10" s="20">
+        <f t="shared" si="2"/>
+        <v>2.970716422399998</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="18">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="B11" s="19">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C11" s="14">
+        <f>C2*POWER(B11,A10)</f>
+        <v>4.7158953820000029</v>
+      </c>
+      <c r="D11" s="14">
+        <f>C2*POWER(B11,A10 - L3)</f>
+        <v>3.5431220000000017</v>
+      </c>
+      <c r="E11" s="19">
+        <v>1.2</v>
+      </c>
+      <c r="F11" s="14">
+        <f>F2*POWER(E11,A11)</f>
+        <v>6.1917364223999991</v>
+      </c>
+      <c r="G11" s="14">
+        <f>F2*POWER(E11,(A11 + L4))</f>
+        <v>7.4300837068799988</v>
+      </c>
+      <c r="H11" s="20">
+        <f t="shared" si="0"/>
+        <v>1.4758410403999962</v>
+      </c>
+      <c r="I11" s="20">
+        <f t="shared" si="2"/>
+        <v>3.8869617068799971</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="18">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="B12" s="19">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C12" s="14">
+        <f>C2*POWER(B12,A11)</f>
+        <v>5.1874849202000037</v>
+      </c>
+      <c r="D12" s="14">
+        <f>C2*POWER(B12,A11 - L3)</f>
+        <v>3.8974342000000024</v>
+      </c>
+      <c r="E12" s="19">
+        <v>1.2</v>
+      </c>
+      <c r="F12" s="14">
+        <f>F2*POWER(E12,A12)</f>
+        <v>7.4300837068799988</v>
+      </c>
+      <c r="G12" s="14">
+        <f>F2*POWER(E12,(A12 + L4))</f>
+        <v>8.9161004482559978</v>
+      </c>
+      <c r="H12" s="20">
+        <f t="shared" si="0"/>
+        <v>2.242598786679995</v>
+      </c>
+      <c r="I12" s="20">
+        <f t="shared" si="2"/>
+        <v>5.0186662482559949</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="18">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="B13" s="19">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C13" s="14">
+        <f>C2*POWER(B13,A12)</f>
+        <v>5.7062334122200049</v>
+      </c>
+      <c r="D13" s="14">
+        <f>C2*POWER(B13,A12 - L3)</f>
+        <v>4.2871776200000022</v>
+      </c>
+      <c r="E13" s="19">
+        <v>1.2</v>
+      </c>
+      <c r="F13" s="14">
+        <f>F2*POWER(E13,A13)</f>
+        <v>8.9161004482559978</v>
+      </c>
+      <c r="G13" s="14">
+        <f>F2*POWER(E13,(A13 + L4))</f>
+        <v>10.699320537907198</v>
+      </c>
+      <c r="H13" s="20">
+        <f t="shared" si="0"/>
+        <v>3.2098670360359929</v>
+      </c>
+      <c r="I13" s="20">
+        <f t="shared" si="2"/>
+        <v>6.4121429179071958</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="18">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="B14" s="19">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C14" s="14">
+        <f>C2*POWER(B14,A13)</f>
+        <v>6.2768567534420052</v>
+      </c>
+      <c r="D14" s="14">
+        <f>C2*POWER(B14,A13 - L3)</f>
+        <v>4.7158953820000029</v>
+      </c>
+      <c r="E14" s="19">
+        <v>1.2</v>
+      </c>
+      <c r="F14" s="14">
+        <f>F2*POWER(E14,A14)</f>
+        <v>10.699320537907198</v>
+      </c>
+      <c r="G14" s="14">
+        <f>F2*POWER(E14,(A14 + L4))</f>
+        <v>12.839184645488636</v>
+      </c>
+      <c r="H14" s="20">
+        <f t="shared" si="0"/>
+        <v>4.4224637844651928</v>
+      </c>
+      <c r="I14" s="20">
+        <f t="shared" si="2"/>
+        <v>8.1232892634886333</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="18">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="B15" s="19">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C15" s="14">
+        <f>C2*POWER(B15,A14)</f>
+        <v>6.9045424287862058</v>
+      </c>
+      <c r="D15" s="14">
+        <f>C2*POWER(B15,A14 - L3)</f>
+        <v>5.1874849202000037</v>
+      </c>
+      <c r="E15" s="19">
+        <v>1.2</v>
+      </c>
+      <c r="F15" s="14">
+        <f>F2*POWER(E15,A15)</f>
+        <v>12.839184645488636</v>
+      </c>
+      <c r="G15" s="14">
+        <f>F2*POWER(E15,(A15 + L4))</f>
+        <v>15.407021574586365</v>
+      </c>
+      <c r="H15" s="20">
+        <f t="shared" si="0"/>
+        <v>5.9346422167024304</v>
+      </c>
+      <c r="I15" s="20">
+        <f t="shared" si="2"/>
+        <v>10.21953665438636</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="18">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="B16" s="19">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C16" s="14">
+        <f>C2*POWER(B16,A15)</f>
+        <v>7.5949966716648278</v>
+      </c>
+      <c r="D16" s="14">
+        <f>C2*POWER(B16,A15 - L3)</f>
+        <v>5.7062334122200049</v>
+      </c>
+      <c r="E16" s="19">
+        <v>1.2</v>
+      </c>
+      <c r="F16" s="14">
+        <f>F2*POWER(E16,A16)</f>
+        <v>15.407021574586365</v>
+      </c>
+      <c r="G16" s="14">
+        <f>F2*POWER(E16,(A16 + L4))</f>
+        <v>18.488425889503635</v>
+      </c>
+      <c r="H16" s="20">
+        <f t="shared" si="0"/>
+        <v>7.8120249029215367</v>
+      </c>
+      <c r="I16" s="20">
+        <f t="shared" si="2"/>
+        <v>12.78219247728363</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="18">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="B17" s="19">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C17" s="14">
+        <f>C2*POWER(B17,A16)</f>
+        <v>8.3544963388313107</v>
+      </c>
+      <c r="D17" s="14">
+        <f>C2*POWER(B17,A16 - L3)</f>
+        <v>6.2768567534420052</v>
+      </c>
+      <c r="E17" s="19">
+        <v>1.2</v>
+      </c>
+      <c r="F17" s="14">
+        <f>F2*POWER(E17,A17)</f>
+        <v>18.488425889503635</v>
+      </c>
+      <c r="G17" s="14">
+        <f>F2*POWER(E17,(A17 + L4))</f>
+        <v>22.186111067404362</v>
+      </c>
+      <c r="H17" s="20">
+        <f t="shared" si="0"/>
+        <v>10.133929550672324</v>
+      </c>
+      <c r="I17" s="20">
+        <f t="shared" si="2"/>
+        <v>15.909254313962357</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="18">
+        <f t="shared" si="1"/>
+        <v>17</v>
+      </c>
+      <c r="B18" s="19">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C18" s="14">
+        <f>C2*POWER(B18,A17)</f>
+        <v>9.1899459727144421</v>
+      </c>
+      <c r="D18" s="14">
+        <f>C2*POWER(B18,A17 - L3)</f>
+        <v>6.9045424287862058</v>
+      </c>
+      <c r="E18" s="19">
+        <v>1.2</v>
+      </c>
+      <c r="F18" s="14">
+        <f>F2*POWER(E18,A18)</f>
+        <v>22.186111067404362</v>
+      </c>
+      <c r="G18" s="14">
+        <f>F2*POWER(E18,(A18 + L4))</f>
+        <v>26.623333280885234</v>
+      </c>
+      <c r="H18" s="20">
+        <f t="shared" si="0"/>
+        <v>12.996165094689919</v>
+      </c>
+      <c r="I18" s="20">
+        <f t="shared" si="2"/>
+        <v>19.718790852099026</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="18">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="B19" s="19">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C19" s="14">
+        <f>C2*POWER(B19,A18)</f>
+        <v>10.108940569985887</v>
+      </c>
+      <c r="D19" s="14">
+        <f>C2*POWER(B19,A18 - L3)</f>
+        <v>7.5949966716648278</v>
+      </c>
+      <c r="E19" s="19">
+        <v>1.2</v>
+      </c>
+      <c r="F19" s="14">
+        <f>F2*POWER(E19,A19)</f>
+        <v>26.623333280885234</v>
+      </c>
+      <c r="G19" s="14">
+        <f>F2*POWER(E19,(A19 + L4))</f>
+        <v>31.947999937062281</v>
+      </c>
+      <c r="H19" s="20">
+        <f t="shared" si="0"/>
+        <v>16.514392710899347</v>
+      </c>
+      <c r="I19" s="20">
+        <f t="shared" si="2"/>
+        <v>24.353003265397454</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="18">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+      <c r="B20" s="19">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C20" s="14">
+        <f>C2*POWER(B20,A19)</f>
+        <v>11.119834626984476</v>
+      </c>
+      <c r="D20" s="14">
+        <f>C2*POWER(B20,A19 - L3)</f>
+        <v>8.3544963388313107</v>
+      </c>
+      <c r="E20" s="19">
+        <v>1.2</v>
+      </c>
+      <c r="F20" s="14">
+        <f>F2*POWER(E20,A20)</f>
+        <v>31.947999937062281</v>
+      </c>
+      <c r="G20" s="14">
+        <f>F2*POWER(E20,(A20 + L4))</f>
+        <v>38.337599924474738</v>
+      </c>
+      <c r="H20" s="20">
+        <f t="shared" si="0"/>
+        <v>20.828165310077807</v>
+      </c>
+      <c r="I20" s="20">
+        <f t="shared" si="2"/>
+        <v>29.983103585643427</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="18">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="B21" s="19">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C21" s="14">
+        <f>C2*POWER(B21,A20)</f>
+        <v>12.231818089682926</v>
+      </c>
+      <c r="D21" s="14">
+        <f>C2*POWER(B21,A20 - L3)</f>
+        <v>9.1899459727144421</v>
+      </c>
+      <c r="E21" s="19">
+        <v>1.2</v>
+      </c>
+      <c r="F21" s="14">
+        <f>F2*POWER(E21,A21)</f>
+        <v>38.337599924474738</v>
+      </c>
+      <c r="G21" s="14">
+        <f>F2*POWER(E21,(A21 + L4))</f>
+        <v>46.005119909369682</v>
+      </c>
+      <c r="H21" s="20">
+        <f t="shared" si="0"/>
+        <v>26.105781834791813</v>
+      </c>
+      <c r="I21" s="20">
+        <f t="shared" si="2"/>
+        <v>36.815173936655242</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="18">
+        <f t="shared" si="1"/>
+        <v>21</v>
+      </c>
+      <c r="B22" s="19">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C22" s="14">
+        <f>C2*POWER(B22,A21)</f>
+        <v>13.454999898651218</v>
+      </c>
+      <c r="D22" s="14">
+        <f>C2*POWER(B22,A21 - L3)</f>
+        <v>10.108940569985887</v>
+      </c>
+      <c r="E22" s="19">
+        <v>1.2</v>
+      </c>
+      <c r="F22" s="14">
+        <f>F2*POWER(E22,A22)</f>
+        <v>46.005119909369682</v>
+      </c>
+      <c r="G22" s="14">
+        <f>F2*POWER(E22,(A22 + L4))</f>
+        <v>55.206143891243613</v>
+      </c>
+      <c r="H22" s="20">
+        <f t="shared" si="0"/>
+        <v>32.550120010718466</v>
+      </c>
+      <c r="I22" s="20">
+        <f t="shared" si="2"/>
+        <v>45.097203321257723</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="18">
+        <f t="shared" si="1"/>
+        <v>22</v>
+      </c>
+      <c r="B23" s="19">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C23" s="14">
+        <f>C2*POWER(B23,A22)</f>
+        <v>14.800499888516342</v>
+      </c>
+      <c r="D23" s="14">
+        <f>C2*POWER(B23,A22 - L3)</f>
+        <v>11.119834626984476</v>
+      </c>
+      <c r="E23" s="19">
+        <v>1.2</v>
+      </c>
+      <c r="F23" s="14">
+        <f>F2*POWER(E23,A23)</f>
+        <v>55.206143891243613</v>
+      </c>
+      <c r="G23" s="14">
+        <f>F2*POWER(E23,(A23 + L4))</f>
+        <v>66.247372669492336</v>
+      </c>
+      <c r="H23" s="20">
+        <f t="shared" si="0"/>
+        <v>40.405644002727271</v>
+      </c>
+      <c r="I23" s="20">
+        <f t="shared" si="2"/>
+        <v>55.127538042507858</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="18">
+        <f t="shared" si="1"/>
+        <v>23</v>
+      </c>
+      <c r="B24" s="19">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C24" s="14">
+        <f>C2*POWER(B24,A23)</f>
+        <v>16.280549877367978</v>
+      </c>
+      <c r="D24" s="14">
+        <f>C2*POWER(B24,A23 - L3)</f>
+        <v>12.231818089682926</v>
+      </c>
+      <c r="E24" s="19">
+        <v>1.2</v>
+      </c>
+      <c r="F24" s="14">
+        <f>F2*POWER(E24,A24)</f>
+        <v>66.247372669492336</v>
+      </c>
+      <c r="G24" s="14">
+        <f>F2*POWER(E24,(A24 + L4))</f>
+        <v>79.4968472033908</v>
+      </c>
+      <c r="H24" s="20">
+        <f t="shared" si="0"/>
+        <v>49.966822792124361</v>
+      </c>
+      <c r="I24" s="20">
+        <f t="shared" si="2"/>
+        <v>67.265029113707868</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="18">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+      <c r="B25" s="19">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C25" s="14">
+        <f>C2*POWER(B25,A24)</f>
+        <v>17.908604865104778</v>
+      </c>
+      <c r="D25" s="14">
+        <f>C2*POWER(B25,A24 - L3)</f>
+        <v>13.454999898651218</v>
+      </c>
+      <c r="E25" s="19">
+        <v>1.2</v>
+      </c>
+      <c r="F25" s="14">
+        <f>F2*POWER(E25,A25)</f>
+        <v>79.4968472033908</v>
+      </c>
+      <c r="G25" s="14">
+        <f>F2*POWER(E25,(A25 + L4))</f>
+        <v>95.396216644068971</v>
+      </c>
+      <c r="H25" s="20">
+        <f t="shared" si="0"/>
+        <v>61.588242338286022</v>
+      </c>
+      <c r="I25" s="20">
+        <f t="shared" si="2"/>
+        <v>81.941216745417748</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="18">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="B26" s="19">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C26" s="14">
+        <f>C2*POWER(B26,A25)</f>
+        <v>19.699465351615252</v>
+      </c>
+      <c r="D26" s="14">
+        <f>C2*POWER(B26,A25 - L3)</f>
+        <v>14.800499888516342</v>
+      </c>
+      <c r="E26" s="19">
+        <v>1.2</v>
+      </c>
+      <c r="F26" s="14">
+        <f>F2*POWER(E26,A26)</f>
+        <v>95.396216644068971</v>
+      </c>
+      <c r="G26" s="14">
+        <f>F2*POWER(E26,(A26 + L4))</f>
+        <v>114.47545997288276</v>
+      </c>
+      <c r="H26" s="20">
+        <f t="shared" si="0"/>
+        <v>75.696751292453712</v>
+      </c>
+      <c r="I26" s="20">
+        <f t="shared" si="2"/>
+        <v>99.674960084366418</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="18">
+        <f t="shared" si="1"/>
+        <v>26</v>
+      </c>
+      <c r="B27" s="19">
+        <v>1.2</v>
+      </c>
+      <c r="C27" s="14">
+        <f>C26*POWER(B27,A26)</f>
+        <v>1879.2544644550189</v>
+      </c>
+      <c r="D27" s="14">
+        <f>D26*POWER(B27,A26 - L3)</f>
+        <v>817.07852650776817</v>
+      </c>
+      <c r="E27" s="19">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F27" s="14">
+        <f>F26*POWER(E27,A27)</f>
+        <v>1136.9489509952869</v>
+      </c>
+      <c r="G27" s="14">
+        <f>G26*POWER(E27,(A27 + L4))</f>
+        <v>1500.7726153137787</v>
+      </c>
+      <c r="H27" s="20">
+        <f t="shared" si="0"/>
+        <v>-742.30551345973208</v>
+      </c>
+      <c r="I27" s="20">
+        <f t="shared" si="2"/>
+        <v>683.69408880601054</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="18">
+        <f t="shared" si="1"/>
+        <v>27</v>
+      </c>
+      <c r="B28" s="19">
+        <v>1.2</v>
+      </c>
+      <c r="C28" s="14">
+        <f>C26*POWER(B28,A27)</f>
+        <v>2255.1053573460226</v>
+      </c>
+      <c r="D28" s="14">
+        <f>D26*POWER(B28,A27 - L3)</f>
+        <v>980.49423180932183</v>
+      </c>
+      <c r="E28" s="19">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F28" s="14">
+        <f>F26*POWER(E28,A28)</f>
+        <v>1250.6438460948157</v>
+      </c>
+      <c r="G28" s="14">
+        <f>G26*POWER(E28,(A28 + L4))</f>
+        <v>1650.8498768451566</v>
+      </c>
+      <c r="H28" s="20">
+        <f t="shared" si="0"/>
+        <v>-1004.461511251207</v>
+      </c>
+      <c r="I28" s="20">
+        <f t="shared" si="2"/>
+        <v>670.35564503583475</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="18">
+        <f t="shared" si="1"/>
+        <v>28</v>
+      </c>
+      <c r="B29" s="19">
+        <v>1.2</v>
+      </c>
+      <c r="C29" s="14">
+        <f>C26*POWER(B29,A28)</f>
+        <v>2706.126428815227</v>
+      </c>
+      <c r="D29" s="14">
+        <f>D26*POWER(B29,A28 - L3)</f>
+        <v>1176.5930781711861</v>
+      </c>
+      <c r="E29" s="19">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F29" s="14">
+        <f>F26*POWER(E29,A29)</f>
+        <v>1375.7082307042972</v>
+      </c>
+      <c r="G29" s="14">
+        <f>G26*POWER(E29,(A29 + L4))</f>
+        <v>1815.9348645296723</v>
+      </c>
+      <c r="H29" s="20">
+        <f t="shared" si="0"/>
+        <v>-1330.4181981109298</v>
+      </c>
+      <c r="I29" s="20">
+        <f t="shared" si="2"/>
+        <v>639.34178635848616</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="18">
+        <f t="shared" si="1"/>
+        <v>29</v>
+      </c>
+      <c r="B30" s="19">
+        <v>1.2</v>
+      </c>
+      <c r="C30" s="14">
+        <f>C26*POWER(B30,A29)</f>
+        <v>3247.3517145782725</v>
+      </c>
+      <c r="D30" s="14">
+        <f>D26*POWER(B30,A29 - L3)</f>
+        <v>1411.9116938054235</v>
+      </c>
+      <c r="E30" s="19">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F30" s="14">
+        <f>F26*POWER(E30,A30)</f>
+        <v>1513.2790537747269</v>
+      </c>
+      <c r="G30" s="14">
+        <f>G26*POWER(E30,(A30 + L4))</f>
+        <v>1997.5283509826397</v>
+      </c>
+      <c r="H30" s="20">
+        <f t="shared" si="0"/>
+        <v>-1734.0726608035457</v>
+      </c>
+      <c r="I30" s="20">
+        <f t="shared" si="2"/>
+        <v>585.61665717721621</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="18">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="B31" s="19">
+        <v>1.2</v>
+      </c>
+      <c r="C31" s="14">
+        <f>C26*POWER(B31,A30)</f>
+        <v>3896.8220574939269</v>
+      </c>
+      <c r="D31" s="14">
+        <f>D26*POWER(B31,A30 - L3)</f>
+        <v>1694.2940325665081</v>
+      </c>
+      <c r="E31" s="19">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F31" s="14">
+        <f>F26*POWER(E31,A31)</f>
+        <v>1664.6069591522</v>
+      </c>
+      <c r="G31" s="14">
+        <f>G26*POWER(E31,(A31 + L4))</f>
+        <v>2197.2811860809038</v>
+      </c>
+      <c r="H31" s="20">
+        <f t="shared" si="0"/>
+        <v>-2232.2150983417268</v>
+      </c>
+      <c r="I31" s="20">
+        <f t="shared" si="2"/>
+        <v>502.98715351439569</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="18">
+        <f t="shared" si="1"/>
+        <v>31</v>
+      </c>
+      <c r="B32" s="19">
+        <v>1.2</v>
+      </c>
+      <c r="C32" s="14">
+        <f>C26*POWER(B32,A31)</f>
+        <v>4676.1864689927115</v>
+      </c>
+      <c r="D32" s="14">
+        <f>D26*POWER(B32,A31 - L3)</f>
+        <v>2033.1528390798098</v>
+      </c>
+      <c r="E32" s="19">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F32" s="14">
+        <f>F26*POWER(E32,A32)</f>
+        <v>1831.06765506742</v>
+      </c>
+      <c r="G32" s="14">
+        <f>G26*POWER(E32,(A32 + L4))</f>
+        <v>2417.0093046889942</v>
+      </c>
+      <c r="H32" s="20">
+        <f t="shared" si="0"/>
+        <v>-2845.1188139252918</v>
+      </c>
+      <c r="I32" s="20">
+        <f t="shared" si="2"/>
+        <v>383.8564656091844</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="18">
+        <f t="shared" si="1"/>
+        <v>32</v>
+      </c>
+      <c r="B33" s="19">
+        <v>1.2</v>
+      </c>
+      <c r="C33" s="14">
+        <f>C26*POWER(B33,A32)</f>
+        <v>5611.4237627912544</v>
+      </c>
+      <c r="D33" s="14">
+        <f>D26*POWER(B33,A32 - L3)</f>
+        <v>2439.7834068957718</v>
+      </c>
+      <c r="E33" s="19">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F33" s="14">
+        <f>F26*POWER(E33,A33)</f>
+        <v>2014.174420574162</v>
+      </c>
+      <c r="G33" s="14">
+        <f>G26*POWER(E33,(A33 + L4))</f>
+        <v>2658.7102351578937</v>
+      </c>
+      <c r="H33" s="20">
+        <f t="shared" si="0"/>
+        <v>-3597.2493422170924</v>
+      </c>
+      <c r="I33" s="20">
+        <f t="shared" si="2"/>
+        <v>218.92682826212194</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" s="18">
+        <f t="shared" si="1"/>
+        <v>33</v>
+      </c>
+      <c r="B34" s="19">
+        <v>1.2</v>
+      </c>
+      <c r="C34" s="14">
+        <f>C26*POWER(B34,A33)</f>
+        <v>6733.7085153495036</v>
+      </c>
+      <c r="D34" s="14">
+        <f>D26*POWER(B34,A33 - L3)</f>
+        <v>2927.7400882749262</v>
+      </c>
+      <c r="E34" s="19">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F34" s="14">
+        <f>F26*POWER(E34,A34)</f>
+        <v>2215.5918626315784</v>
+      </c>
+      <c r="G34" s="14">
+        <f>G26*POWER(E34,(A34 + L4))</f>
+        <v>2924.5812586736834</v>
+      </c>
+      <c r="H34" s="20">
+        <f t="shared" ref="H34:H65" si="3">F34-C34</f>
+        <v>-4518.1166527179248</v>
+      </c>
+      <c r="I34" s="20">
+        <f t="shared" si="2"/>
+        <v>-3.1588296012428145</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" s="18">
+        <f t="shared" si="1"/>
+        <v>34</v>
+      </c>
+      <c r="B35" s="19">
+        <v>1.2</v>
+      </c>
+      <c r="C35" s="14">
+        <f>C26*POWER(B35,A34)</f>
+        <v>8080.4502184194043</v>
+      </c>
+      <c r="D35" s="14">
+        <f>D26*POWER(B35,A34 - L3)</f>
+        <v>3513.2881059299111</v>
+      </c>
+      <c r="E35" s="19">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F35" s="14">
+        <f>F26*POWER(E35,A35)</f>
+        <v>2437.1510488947365</v>
+      </c>
+      <c r="G35" s="14">
+        <f>G26*POWER(E35,(A35 + L4))</f>
+        <v>3217.0393845410526</v>
+      </c>
+      <c r="H35" s="20">
+        <f t="shared" si="3"/>
+        <v>-5643.2991695246674</v>
+      </c>
+      <c r="I35" s="20">
+        <f t="shared" si="2"/>
+        <v>-296.24872138885848</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" s="18">
+        <f t="shared" si="1"/>
+        <v>35</v>
+      </c>
+      <c r="B36" s="19">
+        <v>1.2</v>
+      </c>
+      <c r="C36" s="14">
+        <f>C26*POWER(B36,A35)</f>
+        <v>9696.5402621032845</v>
+      </c>
+      <c r="D36" s="14">
+        <f>D26*POWER(B36,A35 - L3)</f>
+        <v>4215.9457271158926</v>
+      </c>
+      <c r="E36" s="19">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F36" s="14">
+        <f>F26*POWER(E36,A36)</f>
+        <v>2680.8661537842104</v>
+      </c>
+      <c r="G36" s="14">
+        <f>G26*POWER(E36,(A36 + L4))</f>
+        <v>3538.7433229951575</v>
+      </c>
+      <c r="H36" s="20">
+        <f t="shared" si="3"/>
+        <v>-7015.6741083190736</v>
+      </c>
+      <c r="I36" s="20">
+        <f t="shared" si="2"/>
+        <v>-677.20240412073508</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" s="18">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+      <c r="B37" s="19">
+        <v>1.2</v>
+      </c>
+      <c r="C37" s="14">
+        <f>C26*POWER(B37,A36)</f>
+        <v>11635.848314523942</v>
+      </c>
+      <c r="D37" s="14">
+        <f>D26*POWER(B37,A36 - L3)</f>
+        <v>5059.1348725390708</v>
+      </c>
+      <c r="E37" s="19">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F37" s="14">
+        <f>F26*POWER(E37,A37)</f>
+        <v>2948.9527691626313</v>
+      </c>
+      <c r="G37" s="14">
+        <f>G26*POWER(E37,(A37 + L4))</f>
+        <v>3892.6176552946736</v>
+      </c>
+      <c r="H37" s="20">
+        <f t="shared" si="3"/>
+        <v>-8686.8955453613107</v>
+      </c>
+      <c r="I37" s="20">
+        <f t="shared" si="2"/>
+        <v>-1166.5172172443972</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" s="18">
+        <f>A37+1</f>
+        <v>37</v>
+      </c>
+      <c r="B38" s="19">
+        <v>1.2</v>
+      </c>
+      <c r="C38" s="14">
+        <f>C26*POWER(B38,A37)</f>
+        <v>13963.01797742873</v>
+      </c>
+      <c r="D38" s="14">
+        <f>D26*POWER(B38,A37 - L3)</f>
+        <v>6070.9618470468849</v>
+      </c>
+      <c r="E38" s="19">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F38" s="14">
+        <f>F26*POWER(E38,A38)</f>
+        <v>3243.8480460788946</v>
+      </c>
+      <c r="G38" s="14">
+        <f>G26*POWER(E38,(A38 + L4))</f>
+        <v>4281.8794208241416</v>
+      </c>
+      <c r="H38" s="20">
+        <f t="shared" si="3"/>
+        <v>-10719.169931349836</v>
+      </c>
+      <c r="I38" s="20">
+        <f t="shared" si="2"/>
+        <v>-1789.0824262227434</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" s="18">
+        <f t="shared" si="1"/>
+        <v>38</v>
+      </c>
+      <c r="B39" s="19">
+        <v>1.2</v>
+      </c>
+      <c r="C39" s="14">
+        <f>C26*POWER(B39,A38)</f>
+        <v>16755.621572914479</v>
+      </c>
+      <c r="D39" s="14">
+        <f>D26*POWER(B39,A38 - L3)</f>
+        <v>7285.1542164562616</v>
+      </c>
+      <c r="E39" s="19">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F39" s="14">
+        <f>F26*POWER(E39,A39)</f>
+        <v>3568.2328506867848</v>
+      </c>
+      <c r="G39" s="14">
+        <f>G26*POWER(E39,(A39 + L4))</f>
+        <v>4710.0673629065559</v>
+      </c>
+      <c r="H39" s="20">
+        <f t="shared" si="3"/>
+        <v>-13187.388722227694</v>
+      </c>
+      <c r="I39" s="20">
+        <f t="shared" si="2"/>
+        <v>-2575.0868535497057</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" s="18">
+        <f t="shared" si="1"/>
+        <v>39</v>
+      </c>
+      <c r="B40" s="19">
+        <v>1.2</v>
+      </c>
+      <c r="C40" s="14">
+        <f>C26*POWER(B40,A39)</f>
+        <v>20106.745887497371</v>
+      </c>
+      <c r="D40" s="14">
+        <f>D26*POWER(B40,A39 - L3)</f>
+        <v>8742.1850597475132</v>
+      </c>
+      <c r="E40" s="19">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F40" s="14">
+        <f>F26*POWER(E40,A40)</f>
+        <v>3925.0561357554639</v>
+      </c>
+      <c r="G40" s="14">
+        <f>G26*POWER(E40,(A40 + L4))</f>
+        <v>5181.0740991972116</v>
+      </c>
+      <c r="H40" s="20">
+        <f t="shared" si="3"/>
+        <v>-16181.689751741907</v>
+      </c>
+      <c r="I40" s="20">
+        <f t="shared" si="2"/>
+        <v>-3561.1109605503016</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" s="18">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="B41" s="19">
+        <v>1.2</v>
+      </c>
+      <c r="C41" s="14">
+        <f>C26*POWER(B41,A40)</f>
+        <v>24128.095064996844</v>
+      </c>
+      <c r="D41" s="14">
+        <f>D26*POWER(B41,A40 - L3)</f>
+        <v>10490.622071697017</v>
+      </c>
+      <c r="E41" s="19">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F41" s="14">
+        <f>F26*POWER(E41,A41)</f>
+        <v>4317.5617493310092</v>
+      </c>
+      <c r="G41" s="14">
+        <f>G26*POWER(E41,(A41 + L4))</f>
+        <v>5699.1815091169328</v>
+      </c>
+      <c r="H41" s="20">
+        <f t="shared" si="3"/>
+        <v>-19810.533315665834</v>
+      </c>
+      <c r="I41" s="20">
+        <f t="shared" si="2"/>
+        <v>-4791.4405625800837</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" s="18">
+        <f t="shared" si="1"/>
+        <v>41</v>
+      </c>
+      <c r="B42" s="19">
+        <v>1.2</v>
+      </c>
+      <c r="C42" s="14">
+        <f>C26*POWER(B42,A41)</f>
+        <v>28953.714077996214</v>
+      </c>
+      <c r="D42" s="14">
+        <f>D26*POWER(B42,A41 - L3)</f>
+        <v>12588.74648603642</v>
+      </c>
+      <c r="E42" s="19">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F42" s="14">
+        <f>F26*POWER(E42,A42)</f>
+        <v>4749.3179242641108</v>
+      </c>
+      <c r="G42" s="14">
+        <f>G26*POWER(E42,(A42 + L4))</f>
+        <v>6269.0996600286262</v>
+      </c>
+      <c r="H42" s="20">
+        <f t="shared" si="3"/>
+        <v>-24204.396153732101</v>
+      </c>
+      <c r="I42" s="20">
+        <f t="shared" si="2"/>
+        <v>-6319.6468260077936</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" s="18">
+        <f t="shared" si="1"/>
+        <v>42</v>
+      </c>
+      <c r="B43" s="19">
+        <v>1.2</v>
+      </c>
+      <c r="C43" s="14">
+        <f>C26*POWER(B43,A42)</f>
+        <v>34744.456893595452</v>
+      </c>
+      <c r="D43" s="14">
+        <f>D26*POWER(B43,A42 - L3)</f>
+        <v>15106.495783243703</v>
+      </c>
+      <c r="E43" s="19">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F43" s="14">
+        <f>F26*POWER(E43,A43)</f>
+        <v>5224.2497166905223</v>
+      </c>
+      <c r="G43" s="14">
+        <f>G26*POWER(E43,(A43 + L4))</f>
+        <v>6896.0096260314904</v>
+      </c>
+      <c r="H43" s="20">
+        <f t="shared" si="3"/>
+        <v>-29520.207176904929</v>
+      </c>
+      <c r="I43" s="20">
+        <f t="shared" si="2"/>
+        <v>-8210.4861572122136</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44" s="18">
+        <f t="shared" si="1"/>
+        <v>43</v>
+      </c>
+      <c r="B44" s="19">
+        <v>1.2</v>
+      </c>
+      <c r="C44" s="14">
+        <f>C26*POWER(B44,A43)</f>
+        <v>41693.34827231455</v>
+      </c>
+      <c r="D44" s="14">
+        <f>D26*POWER(B44,A43 - L3)</f>
+        <v>18127.794939892443</v>
+      </c>
+      <c r="E44" s="19">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F44" s="14">
+        <f>F26*POWER(E44,A44)</f>
+        <v>5746.6746883595761</v>
+      </c>
+      <c r="G44" s="14">
+        <f>G26*POWER(E44,(A44 + L4))</f>
+        <v>7585.6105886346395</v>
+      </c>
+      <c r="H44" s="20">
+        <f t="shared" si="3"/>
+        <v>-35946.673583954973</v>
+      </c>
+      <c r="I44" s="20">
+        <f t="shared" si="2"/>
+        <v>-10542.184351257803</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45" s="18">
+        <f t="shared" si="1"/>
+        <v>44</v>
+      </c>
+      <c r="B45" s="19">
+        <v>1.2</v>
+      </c>
+      <c r="C45" s="14">
+        <f>C26*POWER(B45,A44)</f>
+        <v>50032.017926777451</v>
+      </c>
+      <c r="D45" s="14">
+        <f>D26*POWER(B45,A44 - L3)</f>
+        <v>21753.353927870932</v>
+      </c>
+      <c r="E45" s="19">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F45" s="14">
+        <f>F26*POWER(E45,A45)</f>
+        <v>6321.3421571955332</v>
+      </c>
+      <c r="G45" s="14">
+        <f>G26*POWER(E45,(A45 + L4))</f>
+        <v>8344.171647498104</v>
+      </c>
+      <c r="H45" s="20">
+        <f t="shared" si="3"/>
+        <v>-43710.675769581918</v>
+      </c>
+      <c r="I45" s="20">
+        <f t="shared" si="2"/>
+        <v>-13409.182280372828</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46" s="18">
+        <f t="shared" si="1"/>
+        <v>45</v>
+      </c>
+      <c r="B46" s="19">
+        <v>1.2</v>
+      </c>
+      <c r="C46" s="14">
+        <f>C26*POWER(B46,A45)</f>
+        <v>60038.42151213294</v>
+      </c>
+      <c r="D46" s="14">
+        <f>D26*POWER(B46,A45 - L3)</f>
+        <v>26104.024713445117</v>
+      </c>
+      <c r="E46" s="19">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F46" s="14">
+        <f>F26*POWER(E46,A46)</f>
+        <v>6953.4763729150873</v>
+      </c>
+      <c r="G46" s="14">
+        <f>G26*POWER(E46,(A46 + L4))</f>
+        <v>9178.5888122479155</v>
+      </c>
+      <c r="H46" s="20">
+        <f t="shared" si="3"/>
+        <v>-53084.945139217853</v>
+      </c>
+      <c r="I46" s="20">
+        <f t="shared" si="2"/>
+        <v>-16925.435901197201</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47" s="18">
+        <f t="shared" si="1"/>
+        <v>46</v>
+      </c>
+      <c r="B47" s="19">
+        <v>1.2</v>
+      </c>
+      <c r="C47" s="14">
+        <f>C26*POWER(B47,A46)</f>
+        <v>72046.105814559531</v>
+      </c>
+      <c r="D47" s="14">
+        <f>D26*POWER(B47,A46 - L3)</f>
+        <v>31324.829656134141</v>
+      </c>
+      <c r="E47" s="19">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F47" s="14">
+        <f>F26*POWER(E47,A47)</f>
+        <v>7648.8240102065965</v>
+      </c>
+      <c r="G47" s="14">
+        <f>G26*POWER(E47,(A47 + L4))</f>
+        <v>10096.447693472708</v>
+      </c>
+      <c r="H47" s="20">
+        <f t="shared" si="3"/>
+        <v>-64397.281804352933</v>
+      </c>
+      <c r="I47" s="20">
+        <f t="shared" si="2"/>
+        <v>-21228.381962661435</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48" s="18">
+        <f t="shared" si="1"/>
+        <v>47</v>
+      </c>
+      <c r="B48" s="19">
+        <v>1.2</v>
+      </c>
+      <c r="C48" s="14">
+        <f>C26*POWER(B48,A47)</f>
+        <v>86455.326977471428</v>
+      </c>
+      <c r="D48" s="14">
+        <f>D26*POWER(B48,A47 - L3)</f>
+        <v>37589.795587360968</v>
+      </c>
+      <c r="E48" s="19">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F48" s="14">
+        <f>F26*POWER(E48,A48)</f>
+        <v>8413.7064112272565</v>
+      </c>
+      <c r="G48" s="14">
+        <f>G26*POWER(E48,(A48 + L4))</f>
+        <v>11106.092462819977</v>
+      </c>
+      <c r="H48" s="20">
+        <f t="shared" si="3"/>
+        <v>-78041.620566244179</v>
+      </c>
+      <c r="I48" s="20">
+        <f t="shared" si="2"/>
+        <v>-26483.703124540989</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A49" s="18">
+        <f t="shared" si="1"/>
+        <v>48</v>
+      </c>
+      <c r="B49" s="19">
+        <v>1.2</v>
+      </c>
+      <c r="C49" s="14">
+        <f>C26*POWER(B49,A48)</f>
+        <v>103746.39237296571</v>
+      </c>
+      <c r="D49" s="14">
+        <f>D26*POWER(B49,A48 - L3)</f>
+        <v>45107.754704833162</v>
+      </c>
+      <c r="E49" s="19">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F49" s="14">
+        <f>F26*POWER(E49,A49)</f>
+        <v>9255.0770523499814</v>
+      </c>
+      <c r="G49" s="14">
+        <f>G26*POWER(E49,(A49 + L4))</f>
+        <v>12216.701709101977</v>
+      </c>
+      <c r="H49" s="20">
+        <f t="shared" si="3"/>
+        <v>-94491.315320615729</v>
+      </c>
+      <c r="I49" s="20">
+        <f t="shared" si="2"/>
+        <v>-32891.052995731181</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A50" s="18">
+        <f t="shared" si="1"/>
+        <v>49</v>
+      </c>
+      <c r="B50" s="19">
+        <v>1.2</v>
+      </c>
+      <c r="C50" s="14">
+        <f>C26*POWER(B50,A49)</f>
+        <v>124495.67084755884</v>
+      </c>
+      <c r="D50" s="14">
+        <f>D26*POWER(B50,A49 - L3)</f>
+        <v>54129.305645799795</v>
+      </c>
+      <c r="E50" s="19">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F50" s="14">
+        <f>F26*POWER(E50,A50)</f>
+        <v>10180.584757584982</v>
+      </c>
+      <c r="G50" s="14">
+        <f>G26*POWER(E50,(A50 + L4))</f>
+        <v>13438.371880012175</v>
+      </c>
+      <c r="H50" s="20">
+        <f t="shared" si="3"/>
+        <v>-114315.08608997386</v>
+      </c>
+      <c r="I50" s="20">
+        <f t="shared" si="2"/>
+        <v>-40690.933765787617</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A51" s="18">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="B51" s="19">
+        <v>1.2</v>
+      </c>
+      <c r="C51" s="14">
+        <f>C26*POWER(B51,A50)</f>
+        <v>149394.80501707061</v>
+      </c>
+      <c r="D51" s="14">
+        <f>D26*POWER(B51,A50 - L3)</f>
+        <v>64955.16677495974</v>
+      </c>
+      <c r="E51" s="19">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F51" s="14">
+        <f>F26*POWER(E51,A51)</f>
+        <v>11198.64323334348</v>
+      </c>
+      <c r="G51" s="14">
+        <f>G26*POWER(E51,(A51 + L4))</f>
+        <v>14782.209068013395</v>
+      </c>
+      <c r="H51" s="20">
+        <f t="shared" si="3"/>
+        <v>-138196.16178372712</v>
+      </c>
+      <c r="I51" s="20">
+        <f t="shared" si="2"/>
+        <v>-50172.957706946341</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A52" s="18">
+        <f t="shared" si="1"/>
+        <v>51</v>
+      </c>
+      <c r="B52" s="19">
+        <v>1.2250000000000001</v>
+      </c>
+      <c r="C52" s="14">
+        <f>C51*POWER(B52,A51)</f>
+        <v>3811886235.8499222</v>
+      </c>
+      <c r="D52" s="14">
+        <f>D51*POWER(B52,A51 - L3)</f>
+        <v>901591629.69921792</v>
+      </c>
+      <c r="E52" s="19">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F52" s="14">
+        <f>F51*POWER(E52,A52)</f>
+        <v>1446080.108283387</v>
+      </c>
+      <c r="G52" s="14">
+        <f>G51*POWER(E52,(A52 + L4))</f>
+        <v>2099708.3172274781</v>
+      </c>
+      <c r="H52" s="20">
+        <f t="shared" si="3"/>
+        <v>-3810440155.7416387</v>
+      </c>
+      <c r="I52" s="20">
+        <f t="shared" si="2"/>
+        <v>-899491921.38199043</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A53" s="18">
+        <f t="shared" si="1"/>
+        <v>52</v>
+      </c>
+      <c r="B53" s="19">
+        <v>1.2250000000000001</v>
+      </c>
+      <c r="C53" s="14">
+        <f>C51*POWER(B53,A52)</f>
+        <v>4669560638.9161558</v>
+      </c>
+      <c r="D53" s="14">
+        <f>D51*POWER(B53,A52 - L3)</f>
+        <v>1104449746.3815417</v>
+      </c>
+      <c r="E53" s="19">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F53" s="14">
+        <f>F51*POWER(E53,A53)</f>
+        <v>1590688.1191117258</v>
+      </c>
+      <c r="G53" s="14">
+        <f>G51*POWER(E53,(A53 + L4))</f>
+        <v>2309679.1489502261</v>
+      </c>
+      <c r="H53" s="20">
+        <f t="shared" si="3"/>
+        <v>-4667969950.7970438</v>
+      </c>
+      <c r="I53" s="20">
+        <f t="shared" si="2"/>
+        <v>-1102140067.2325914</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A54" s="18">
+        <f t="shared" si="1"/>
+        <v>53</v>
+      </c>
+      <c r="B54" s="19">
+        <v>1.2250000000000001</v>
+      </c>
+      <c r="C54" s="14">
+        <f>C51*POWER(B54,A53)</f>
+        <v>5720211782.6722908</v>
+      </c>
+      <c r="D54" s="14">
+        <f>D51*POWER(B54,A53 - L3)</f>
+        <v>1352950939.317389</v>
+      </c>
+      <c r="E54" s="19">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F54" s="14">
+        <f>F51*POWER(E54,A54)</f>
+        <v>1749756.9310228985</v>
+      </c>
+      <c r="G54" s="14">
+        <f>G51*POWER(E54,(A54 + L4))</f>
+        <v>2540647.0638452489</v>
+      </c>
+      <c r="H54" s="20">
+        <f t="shared" si="3"/>
+        <v>-5718462025.7412682</v>
+      </c>
+      <c r="I54" s="20">
+        <f t="shared" si="2"/>
+        <v>-1350410292.2535439</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A55" s="18">
+        <f t="shared" si="1"/>
+        <v>54</v>
+      </c>
+      <c r="B55" s="19">
+        <v>1.2250000000000001</v>
+      </c>
+      <c r="C55" s="14">
+        <f>C51*POWER(B55,A54)</f>
+        <v>7007259433.7735577</v>
+      </c>
+      <c r="D55" s="14">
+        <f>D51*POWER(B55,A54 - L3)</f>
+        <v>1657364900.6638014</v>
+      </c>
+      <c r="E55" s="19">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F55" s="14">
+        <f>F51*POWER(E55,A55)</f>
+        <v>1924732.6241251887</v>
+      </c>
+      <c r="G55" s="14">
+        <f>G51*POWER(E55,(A55 + L4))</f>
+        <v>2794711.7702297745</v>
+      </c>
+      <c r="H55" s="20">
+        <f t="shared" si="3"/>
+        <v>-7005334701.1494322</v>
+      </c>
+      <c r="I55" s="20">
+        <f t="shared" si="2"/>
+        <v>-1654570188.8935716</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A56" s="18">
+        <f t="shared" si="1"/>
+        <v>55</v>
+      </c>
+      <c r="B56" s="19">
+        <v>1.2250000000000001</v>
+      </c>
+      <c r="C56" s="14">
+        <f>C51*POWER(B56,A55)</f>
+        <v>8583892806.3726091</v>
+      </c>
+      <c r="D56" s="14">
+        <f>D51*POWER(B56,A55 - L3)</f>
+        <v>2030272003.3131571</v>
+      </c>
+      <c r="E56" s="19">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F56" s="14">
+        <f>F51*POWER(E56,A56)</f>
+        <v>2117205.8865377079</v>
+      </c>
+      <c r="G56" s="14">
+        <f>G51*POWER(E56,(A56 + L4))</f>
+        <v>3074182.9472527513</v>
+      </c>
+      <c r="H56" s="20">
+        <f t="shared" si="3"/>
+        <v>-8581775600.4860716</v>
+      </c>
+      <c r="I56" s="20">
+        <f t="shared" si="2"/>
+        <v>-2027197820.3659043</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A57" s="18">
+        <f t="shared" si="1"/>
+        <v>56</v>
+      </c>
+      <c r="B57" s="19">
+        <v>1.2250000000000001</v>
+      </c>
+      <c r="C57" s="14">
+        <f>C51*POWER(B57,A56)</f>
+        <v>10515268687.806446</v>
+      </c>
+      <c r="D57" s="14">
+        <f>D51*POWER(B57,A56 - L3)</f>
+        <v>2487083204.0586176</v>
+      </c>
+      <c r="E57" s="19">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F57" s="14">
+        <f>F51*POWER(E57,A57)</f>
+        <v>2328926.4751914782</v>
+      </c>
+      <c r="G57" s="14">
+        <f>G51*POWER(E57,(A57 + L4))</f>
+        <v>3381601.2419780274</v>
+      </c>
+      <c r="H57" s="20">
+        <f t="shared" si="3"/>
+        <v>-10512939761.331255</v>
+      </c>
+      <c r="I57" s="20">
+        <f t="shared" si="2"/>
+        <v>-2483701602.8166394</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A58" s="18">
+        <f t="shared" si="1"/>
+        <v>57</v>
+      </c>
+      <c r="B58" s="19">
+        <v>1.2250000000000001</v>
+      </c>
+      <c r="C58" s="14">
+        <f>C51*POWER(B58,A57)</f>
+        <v>12881204142.562899</v>
+      </c>
+      <c r="D58" s="14">
+        <f>D51*POWER(B58,A57 - L3)</f>
+        <v>3046676924.971807</v>
+      </c>
+      <c r="E58" s="19">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F58" s="14">
+        <f>F51*POWER(E58,A58)</f>
+        <v>2561819.1227106266</v>
+      </c>
+      <c r="G58" s="14">
+        <f>G51*POWER(E58,(A58 + L4))</f>
+        <v>3719761.3661758299</v>
+      </c>
+      <c r="H58" s="20">
+        <f t="shared" si="3"/>
+        <v>-12878642323.440187</v>
+      </c>
+      <c r="I58" s="20">
+        <f t="shared" si="2"/>
+        <v>-3042957163.6056314</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A59" s="18">
+        <f t="shared" si="1"/>
+        <v>58</v>
+      </c>
+      <c r="B59" s="19">
+        <v>1.2250000000000001</v>
+      </c>
+      <c r="C59" s="14">
+        <f>C51*POWER(B59,A58)</f>
+        <v>15779475074.639551</v>
+      </c>
+      <c r="D59" s="14">
+        <f>D51*POWER(B59,A58 - L3)</f>
+        <v>3732179233.0904641</v>
+      </c>
+      <c r="E59" s="19">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F59" s="14">
+        <f>F51*POWER(E59,A59)</f>
+        <v>2818001.034981689</v>
+      </c>
+      <c r="G59" s="14">
+        <f>G51*POWER(E59,(A59 + L4))</f>
+        <v>4091737.5027934141</v>
+      </c>
+      <c r="H59" s="20">
+        <f t="shared" si="3"/>
+        <v>-15776657073.60457</v>
+      </c>
+      <c r="I59" s="20">
+        <f t="shared" si="2"/>
+        <v>-3728087495.5876708</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A60" s="18">
+        <f t="shared" si="1"/>
+        <v>59</v>
+      </c>
+      <c r="B60" s="19">
+        <v>1.2250000000000001</v>
+      </c>
+      <c r="C60" s="14">
+        <f>C51*POWER(B60,A59)</f>
+        <v>19329856966.433453</v>
+      </c>
+      <c r="D60" s="14">
+        <f>D51*POWER(B60,A59 - L3)</f>
+        <v>4571919560.5358181</v>
+      </c>
+      <c r="E60" s="19">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F60" s="14">
+        <f>F51*POWER(E60,A60)</f>
+        <v>3099801.1384798591</v>
+      </c>
+      <c r="G60" s="14">
+        <f>G51*POWER(E60,(A60 + L4))</f>
+        <v>4500911.2530727545</v>
+      </c>
+      <c r="H60" s="20">
+        <f t="shared" si="3"/>
+        <v>-19326757165.294971</v>
+      </c>
+      <c r="I60" s="20">
+        <f t="shared" si="2"/>
+        <v>-4567418649.2827454</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A61" s="18">
+        <f t="shared" si="1"/>
+        <v>60</v>
+      </c>
+      <c r="B61" s="19">
+        <v>1.2250000000000001</v>
+      </c>
+      <c r="C61" s="14">
+        <f>C51*POWER(B61,A60)</f>
+        <v>23679074783.880981</v>
+      </c>
+      <c r="D61" s="14">
+        <f>D51*POWER(B61,A60 - L3)</f>
+        <v>5600601461.6563787</v>
+      </c>
+      <c r="E61" s="19">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F61" s="14">
+        <f>F51*POWER(E61,A61)</f>
+        <v>3409781.252327844</v>
+      </c>
+      <c r="G61" s="14">
+        <f>G51*POWER(E61,(A61 + L4))</f>
+        <v>4951002.3783800313</v>
+      </c>
+      <c r="H61" s="20">
+        <f t="shared" si="3"/>
+        <v>-23675665002.628654</v>
+      </c>
+      <c r="I61" s="20">
+        <f t="shared" si="2"/>
+        <v>-5595650459.2779989</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A62" s="18">
+        <f t="shared" si="1"/>
+        <v>61</v>
+      </c>
+      <c r="B62" s="19">
+        <v>1.2250000000000001</v>
+      </c>
+      <c r="C62" s="14">
+        <f>C51*POWER(B62,A61)</f>
+        <v>29006866610.2542</v>
+      </c>
+      <c r="D62" s="14">
+        <f>D51*POWER(B62,A61 - L3)</f>
+        <v>6860736790.5290642</v>
+      </c>
+      <c r="E62" s="19">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F62" s="14">
+        <f>F51*POWER(E62,A62)</f>
+        <v>3750759.3775606295</v>
+      </c>
+      <c r="G62" s="14">
+        <f>G51*POWER(E62,(A62 + L4))</f>
+        <v>5446102.6162180351</v>
+      </c>
+      <c r="H62" s="20">
+        <f t="shared" si="3"/>
+        <v>-29003115850.87664</v>
+      </c>
+      <c r="I62" s="20">
+        <f t="shared" si="2"/>
+        <v>-6855290687.9128466</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A63" s="18">
+        <f t="shared" si="1"/>
+        <v>62</v>
+      </c>
+      <c r="B63" s="19">
+        <v>1.2250000000000001</v>
+      </c>
+      <c r="C63" s="14">
+        <f>C51*POWER(B63,A62)</f>
+        <v>35533411597.561409</v>
+      </c>
+      <c r="D63" s="14">
+        <f>D51*POWER(B63,A62 - L3)</f>
+        <v>8404402568.3981047</v>
+      </c>
+      <c r="E63" s="19">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F63" s="14">
+        <f>F51*POWER(E63,A63)</f>
+        <v>4125835.3153166929</v>
+      </c>
+      <c r="G63" s="14">
+        <f>G51*POWER(E63,(A63 + L4))</f>
+        <v>5990712.8778398382</v>
+      </c>
+      <c r="H63" s="20">
+        <f t="shared" si="3"/>
+        <v>-35529285762.246094</v>
+      </c>
+      <c r="I63" s="20">
+        <f t="shared" si="2"/>
+        <v>-8398411855.5202646</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A64" s="18">
+        <f t="shared" si="1"/>
+        <v>63</v>
+      </c>
+      <c r="B64" s="19">
+        <v>1.2250000000000001</v>
+      </c>
+      <c r="C64" s="14">
+        <f>C51*POWER(B64,A63)</f>
+        <v>43528429207.012733</v>
+      </c>
+      <c r="D64" s="14">
+        <f>D51*POWER(B64,A63 - L3)</f>
+        <v>10295393146.28768</v>
+      </c>
+      <c r="E64" s="19">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F64" s="14">
+        <f>F51*POWER(E64,A64)</f>
+        <v>4538418.8468483621</v>
+      </c>
+      <c r="G64" s="14">
+        <f>G51*POWER(E64,(A64 + L4))</f>
+        <v>6589784.1656238222</v>
+      </c>
+      <c r="H64" s="20">
+        <f t="shared" si="3"/>
+        <v>-43523890788.165886</v>
+      </c>
+      <c r="I64" s="20">
+        <f t="shared" si="2"/>
+        <v>-10288803362.122055</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A65" s="18">
+        <f t="shared" si="1"/>
+        <v>64</v>
+      </c>
+      <c r="B65" s="19">
+        <v>1.2250000000000001</v>
+      </c>
+      <c r="C65" s="14">
+        <f>C51*POWER(B65,A64)</f>
+        <v>53322325778.590599</v>
+      </c>
+      <c r="D65" s="14">
+        <f>D51*POWER(B65,A64 - L3)</f>
+        <v>12611856604.202406</v>
+      </c>
+      <c r="E65" s="19">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F65" s="14">
+        <f>F51*POWER(E65,A65)</f>
+        <v>4992260.7315331986</v>
+      </c>
+      <c r="G65" s="14">
+        <f>G51*POWER(E65,(A65 + L4))</f>
+        <v>7248762.5821862053</v>
+      </c>
+      <c r="H65" s="20">
+        <f t="shared" si="3"/>
+        <v>-53317333517.859062</v>
+      </c>
+      <c r="I65" s="20">
+        <f t="shared" si="2"/>
+        <v>-12604607841.62022</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A66" s="18">
+        <f t="shared" si="1"/>
+        <v>65</v>
+      </c>
+      <c r="B66" s="19">
+        <v>1.2250000000000001</v>
+      </c>
+      <c r="C66" s="14">
+        <f>C51*POWER(B66,A65)</f>
+        <v>65319849078.773483</v>
+      </c>
+      <c r="D66" s="14">
+        <f>D51*POWER(B66,A65 - L3)</f>
+        <v>15449524340.147951</v>
+      </c>
+      <c r="E66" s="19">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F66" s="14">
+        <f>F51*POWER(E66,A66)</f>
+        <v>5491486.8046865184</v>
+      </c>
+      <c r="G66" s="14">
+        <f>G51*POWER(E66,(A66 + L4))</f>
+        <v>7973638.8404048262</v>
+      </c>
+      <c r="H66" s="20">
+        <f t="shared" ref="H66:H76" si="4">F66-C66</f>
+        <v>-65314357591.968796</v>
+      </c>
+      <c r="I66" s="20">
+        <f t="shared" si="2"/>
+        <v>-15441550701.307547</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A67" s="18">
+        <f t="shared" si="1"/>
+        <v>66</v>
+      </c>
+      <c r="B67" s="19">
+        <v>1.2250000000000001</v>
+      </c>
+      <c r="C67" s="14">
+        <f>C51*POWER(B67,A66)</f>
+        <v>80016815121.497528</v>
+      </c>
+      <c r="D67" s="14">
+        <f>D51*POWER(B67,A66 - L3)</f>
+        <v>18925667316.681244</v>
+      </c>
+      <c r="E67" s="19">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F67" s="14">
+        <f>F51*POWER(E67,A67)</f>
+        <v>6040635.4851551708</v>
+      </c>
+      <c r="G67" s="14">
+        <f>G51*POWER(E67,(A67 + L4))</f>
+        <v>8771002.7244453114</v>
+      </c>
+      <c r="H67" s="20">
+        <f t="shared" si="4"/>
+        <v>-80010774486.012375</v>
+      </c>
+      <c r="I67" s="20">
+        <f t="shared" si="2"/>
+        <v>-18916896313.956799</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A68" s="18">
+        <f t="shared" ref="A68:A76" si="5">A67+1</f>
+        <v>67</v>
+      </c>
+      <c r="B68" s="19">
+        <v>1.2250000000000001</v>
+      </c>
+      <c r="C68" s="14">
+        <f>C51*POWER(B68,A67)</f>
+        <v>98020598523.834488</v>
+      </c>
+      <c r="D68" s="14">
+        <f>D51*POWER(B68,A67 - L3)</f>
+        <v>23183942462.934525</v>
+      </c>
+      <c r="E68" s="19">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F68" s="14">
+        <f>F51*POWER(E68,A68)</f>
+        <v>6644699.0336706899</v>
+      </c>
+      <c r="G68" s="14">
+        <f>G51*POWER(E68,(A68 + L4))</f>
+        <v>9648102.9968898408</v>
+      </c>
+      <c r="H68" s="20">
+        <f t="shared" si="4"/>
+        <v>-98013953824.800812</v>
+      </c>
+      <c r="I68" s="20">
+        <f t="shared" ref="I68:I76" si="6">G68-D68</f>
+        <v>-23174294359.937634</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A69" s="18">
+        <f t="shared" si="5"/>
+        <v>68</v>
+      </c>
+      <c r="B69" s="19">
+        <v>1.2250000000000001</v>
+      </c>
+      <c r="C69" s="14">
+        <f>C51*POWER(B69,A68)</f>
+        <v>120075233191.69725</v>
+      </c>
+      <c r="D69" s="14">
+        <f>D51*POWER(B69,A68 - L3)</f>
+        <v>28400329517.094795</v>
+      </c>
+      <c r="E69" s="19">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F69" s="14">
+        <f>F51*POWER(E69,A69)</f>
+        <v>7309168.9370377576</v>
+      </c>
+      <c r="G69" s="14">
+        <f>G51*POWER(E69,(A69 + L4))</f>
+        <v>10612913.296578826</v>
+      </c>
+      <c r="H69" s="20">
+        <f t="shared" si="4"/>
+        <v>-120067924022.76021</v>
+      </c>
+      <c r="I69" s="20">
+        <f t="shared" si="6"/>
+        <v>-28389716603.798218</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A70" s="18">
+        <f t="shared" si="5"/>
+        <v>69</v>
+      </c>
+      <c r="B70" s="19">
+        <v>1.2250000000000001</v>
+      </c>
+      <c r="C70" s="14">
+        <f>C51*POWER(B70,A69)</f>
+        <v>147092160659.82913</v>
+      </c>
+      <c r="D70" s="14">
+        <f>D51*POWER(B70,A69 - L3)</f>
+        <v>34790403658.441124</v>
+      </c>
+      <c r="E70" s="19">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F70" s="14">
+        <f>F51*POWER(E70,A70)</f>
+        <v>8040085.8307415349</v>
+      </c>
+      <c r="G70" s="14">
+        <f>G51*POWER(E70,(A70 + L4))</f>
+        <v>11674204.626236711</v>
+      </c>
+      <c r="H70" s="20">
+        <f t="shared" si="4"/>
+        <v>-147084120573.99838</v>
+      </c>
+      <c r="I70" s="20">
+        <f t="shared" si="6"/>
+        <v>-34778729453.814888</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A71" s="18">
+        <f t="shared" si="5"/>
+        <v>70</v>
+      </c>
+      <c r="B71" s="19">
+        <v>1.2250000000000001</v>
+      </c>
+      <c r="C71" s="14">
+        <f>C51*POWER(B71,A70)</f>
+        <v>180187896808.29074</v>
+      </c>
+      <c r="D71" s="14">
+        <f>D51*POWER(B71,A70 - L3)</f>
+        <v>42618244481.590385</v>
+      </c>
+      <c r="E71" s="19">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F71" s="14">
+        <f>F51*POWER(E71,A71)</f>
+        <v>8844094.4138156883</v>
+      </c>
+      <c r="G71" s="14">
+        <f>G51*POWER(E71,(A71 + L4))</f>
+        <v>12841625.088860383</v>
+      </c>
+      <c r="H71" s="20">
+        <f t="shared" si="4"/>
+        <v>-180179052713.87692</v>
+      </c>
+      <c r="I71" s="20">
+        <f t="shared" si="6"/>
+        <v>-42605402856.501526</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A72" s="18">
+        <f t="shared" si="5"/>
+        <v>71</v>
+      </c>
+      <c r="B72" s="19">
+        <v>1.2250000000000001</v>
+      </c>
+      <c r="C72" s="14">
+        <f>C51*POWER(B72,A71)</f>
+        <v>220730173590.15619</v>
+      </c>
+      <c r="D72" s="14">
+        <f>D51*POWER(B72,A71 - L3)</f>
+        <v>52207349489.948227</v>
+      </c>
+      <c r="E72" s="19">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F72" s="14">
+        <f>F51*POWER(E72,A72)</f>
+        <v>9728503.8551972583</v>
+      </c>
+      <c r="G72" s="14">
+        <f>G51*POWER(E72,(A72 + L4))</f>
+        <v>14125787.597746421</v>
+      </c>
+      <c r="H72" s="20">
+        <f t="shared" si="4"/>
+        <v>-220720445086.30099</v>
+      </c>
+      <c r="I72" s="20">
+        <f t="shared" si="6"/>
+        <v>-52193223702.350479</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A73" s="18">
+        <f t="shared" si="5"/>
+        <v>72</v>
+      </c>
+      <c r="B73" s="19">
+        <v>1.2250000000000001</v>
+      </c>
+      <c r="C73" s="14">
+        <f>C51*POWER(B73,A72)</f>
+        <v>270394462647.94131</v>
+      </c>
+      <c r="D73" s="14">
+        <f>D51*POWER(B73,A72 - L3)</f>
+        <v>63954003125.186584</v>
+      </c>
+      <c r="E73" s="19">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F73" s="14">
+        <f>F51*POWER(E73,A73)</f>
+        <v>10701354.240716984</v>
+      </c>
+      <c r="G73" s="14">
+        <f>G51*POWER(E73,(A73 + L4))</f>
+        <v>15538366.357521065</v>
+      </c>
+      <c r="H73" s="20">
+        <f t="shared" si="4"/>
+        <v>-270383761293.70059</v>
+      </c>
+      <c r="I73" s="20">
+        <f t="shared" si="6"/>
+        <v>-63938464758.829063</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A74" s="18">
+        <f t="shared" si="5"/>
+        <v>73</v>
+      </c>
+      <c r="B74" s="19">
+        <v>1.2250000000000001</v>
+      </c>
+      <c r="C74" s="14">
+        <f>C51*POWER(B74,A73)</f>
+        <v>331233216743.72815</v>
+      </c>
+      <c r="D74" s="14">
+        <f>D51*POWER(B74,A73 - L3)</f>
+        <v>78343653828.353577</v>
+      </c>
+      <c r="E74" s="19">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F74" s="14">
+        <f>F51*POWER(E74,A74)</f>
+        <v>11771489.664788684</v>
+      </c>
+      <c r="G74" s="14">
+        <f>G51*POWER(E74,(A74 + L4))</f>
+        <v>17092202.993273169</v>
+      </c>
+      <c r="H74" s="20">
+        <f t="shared" si="4"/>
+        <v>-331221445254.06335</v>
+      </c>
+      <c r="I74" s="20">
+        <f t="shared" si="6"/>
+        <v>-78326561625.360306</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A75" s="18">
+        <f t="shared" si="5"/>
+        <v>74</v>
+      </c>
+      <c r="B75" s="19">
+        <v>1.2250000000000001</v>
+      </c>
+      <c r="C75" s="14">
+        <f>C51*POWER(B75,A74)</f>
+        <v>405760690511.06702</v>
+      </c>
+      <c r="D75" s="14">
+        <f>D51*POWER(B75,A74 - L3)</f>
+        <v>95970975939.733154</v>
+      </c>
+      <c r="E75" s="19">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F75" s="14">
+        <f>F51*POWER(E75,A75)</f>
+        <v>12948638.631267553</v>
+      </c>
+      <c r="G75" s="14">
+        <f>G51*POWER(E75,(A75 + L4))</f>
+        <v>18801423.29260049</v>
+      </c>
+      <c r="H75" s="20">
+        <f t="shared" si="4"/>
+        <v>-405747741872.43573</v>
+      </c>
+      <c r="I75" s="20">
+        <f t="shared" si="6"/>
+        <v>-95952174516.440552</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A76" s="18">
+        <f t="shared" si="5"/>
+        <v>75</v>
+      </c>
+      <c r="B76" s="19">
+        <v>1.2250000000000001</v>
+      </c>
+      <c r="C76" s="14">
+        <f>C51*POWER(B76,A75)</f>
+        <v>497056845876.05719</v>
+      </c>
+      <c r="D76" s="14">
+        <f>D51*POWER(B76,A75 - L3)</f>
+        <v>117564445526.17311</v>
+      </c>
+      <c r="E76" s="19">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F76" s="14">
+        <f>F51*POWER(E76,A76)</f>
+        <v>14243502.49439431</v>
+      </c>
+      <c r="G76" s="14">
+        <f>G51*POWER(E76,(A76 + L4))</f>
+        <v>20681565.621860538</v>
+      </c>
+      <c r="H76" s="20">
+        <f t="shared" si="4"/>
+        <v>-497042602373.56281</v>
+      </c>
+      <c r="I76" s="20">
+        <f t="shared" si="6"/>
+        <v>-117543763960.55125</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>